<commit_message>
added ukb whole dataset fully working run on neuro PM
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20385"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="80" documentId="11_F25DC773A252ABEACE02EC49939867FE5ADE5898" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0CF9ED72-FD32-4ECD-9DF2-F89942EA4A5E}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABEACE02EC49939867FE5ADE5898" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE41EAAB-429E-45F8-A5F0-624BE6C9F74C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5064" yWindow="564" windowWidth="17700" windowHeight="7668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Data Used</t>
   </si>
@@ -79,9 +79,6 @@
     <t>91.8 &amp; 82.8</t>
   </si>
   <si>
-    <t>ukb51139.csv</t>
-  </si>
-  <si>
     <t>&gt; 160/80</t>
   </si>
   <si>
@@ -92,6 +89,18 @@
   </si>
   <si>
     <t>1/0 Overlap</t>
+  </si>
+  <si>
+    <t>ukb51139_subset.csv</t>
+  </si>
+  <si>
+    <t>28012 x 1081</t>
+  </si>
+  <si>
+    <t>94.0 &amp; 81.9</t>
+  </si>
+  <si>
+    <t>66.1 &amp; 53.1</t>
   </si>
 </sst>
 </file>
@@ -421,25 +430,26 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="2.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="2.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" customWidth="1"/>
+    <col min="11" max="11" width="15.109375" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,13 +478,13 @@
         <v>15</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -509,9 +519,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -520,7 +533,7 @@
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -529,7 +542,16 @@
         <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="J3">
+        <v>91</v>
+      </c>
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update job history with new TSR imputation
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABEACE02EC49939867FE5ADE5898" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE41EAAB-429E-45F8-A5F0-624BE6C9F74C}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_F25DC773A252ABEACE02EC49939867FE5ADE5898" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F512CD0B-9F69-4F68-8293-B1627CB5399F}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="564" windowWidth="17700" windowHeight="7668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10032" yWindow="2004" windowWidth="17700" windowHeight="7668" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Data Used</t>
   </si>
@@ -101,6 +101,21 @@
   </si>
   <si>
     <t>66.1 &amp; 53.1</t>
+  </si>
+  <si>
+    <t>TSR</t>
+  </si>
+  <si>
+    <t>85.2 &amp; 80.9</t>
+  </si>
+  <si>
+    <t>50.7 &amp; 45.5</t>
+  </si>
+  <si>
+    <t># Components</t>
+  </si>
+  <si>
+    <t>Alpha</t>
   </si>
 </sst>
 </file>
@@ -427,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,9 +462,10 @@
     <col min="10" max="10" width="10.88671875" customWidth="1"/>
     <col min="11" max="11" width="15.109375" customWidth="1"/>
     <col min="12" max="12" width="14.109375" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,8 +499,14 @@
       <c r="L1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -518,8 +540,11 @@
       <c r="L2" t="s">
         <v>18</v>
       </c>
+      <c r="M2">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -552,6 +577,50 @@
       </c>
       <c r="L3" t="s">
         <v>26</v>
+      </c>
+      <c r="M3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4">
+        <v>105</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M4">
+        <v>17</v>
+      </c>
+      <c r="N4">
+        <v>11.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-compiled matlab script (final version for now), and updated job history list
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Data Used</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>82.4 &amp; 71.7</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -126,7 +129,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,12 +147,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -198,13 +195,16 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -213,11 +213,8 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,25 +518,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="13.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="2.1478571428571427" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="11" width="7.576428571428571" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="12" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
@@ -673,7 +670,7 @@
       <c r="N3" s="5">
         <v>17</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="6">
         <v>47.5</v>
       </c>
     </row>
@@ -718,7 +715,7 @@
       <c r="N4" s="5">
         <v>17</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="6">
         <v>11.8</v>
       </c>
     </row>
@@ -751,7 +748,7 @@
         <v>10</v>
       </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="8">
+      <c r="K5" s="5">
         <v>55</v>
       </c>
       <c r="L5" s="3" t="s">
@@ -760,63 +757,191 @@
       <c r="M5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="N5" s="8">
+      <c r="N5" s="5">
         <v>9</v>
       </c>
       <c r="O5" s="6">
         <v>75.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="8"/>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="5">
+        <v>50</v>
+      </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="8"/>
+      <c r="K6" s="5"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-      <c r="N6" s="8"/>
+      <c r="N6" s="5"/>
       <c r="O6" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3"/>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="8"/>
+      <c r="C7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="5"/>
       <c r="J7" s="3"/>
-      <c r="K7" s="8"/>
+      <c r="K7" s="5"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="5"/>
       <c r="O7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3"/>
+      <c r="A8" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="C8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="I8" s="8"/>
       <c r="J8" s="3"/>
       <c r="K8" s="8"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="6"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="9"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ukb 10% subset working very well, disease model very good
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Data Used</t>
   </si>
   <si>
-    <t>Dimensions</t>
+    <t>Subset Dimensions</t>
   </si>
   <si>
     <t>Column Subset</t>
@@ -49,7 +49,7 @@
     <t>1/0 Overlap</t>
   </si>
   <si>
-    <t>1/2 Overlap</t>
+    <t>2/0 Overlap</t>
   </si>
   <si>
     <t># cPCA</t>
@@ -121,7 +121,22 @@
     <t>82.4 &amp; 71.7</t>
   </si>
   <si>
-    <t/>
+    <t>2802 x 1081</t>
+  </si>
+  <si>
+    <t>62.4 &amp; 42.8</t>
+  </si>
+  <si>
+    <t>-250 &amp; 71.6</t>
+  </si>
+  <si>
+    <t>7003 x 1081</t>
+  </si>
+  <si>
+    <t>25.7 &amp; 10.6</t>
+  </si>
+  <si>
+    <t>17.3 &amp; 9.5</t>
   </si>
 </sst>
 </file>
@@ -129,7 +144,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +162,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -178,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -198,13 +219,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -524,21 +542,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -768,7 +786,7 @@
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -793,104 +811,100 @@
         <v>50</v>
       </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
+      <c r="K6" s="5">
+        <v>429</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="5">
+        <v>16</v>
+      </c>
+      <c r="O6" s="6">
+        <v>57.2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="5"/>
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="5">
+        <v>50</v>
+      </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
+      <c r="K7" s="5">
+        <v>260</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="N7" s="5">
+        <v>15</v>
+      </c>
+      <c r="O7" s="6">
+        <v>68.9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I8" s="8"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="7"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="8"/>
+      <c r="K8" s="7"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="9"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="A9" s="3"/>
       <c r="B9" s="3"/>
-      <c r="C9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I9" s="8"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="7"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="8"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="9"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="3"/>
@@ -901,13 +915,13 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="8"/>
+      <c r="I10" s="7"/>
       <c r="J10" s="3"/>
-      <c r="K10" s="8"/>
+      <c r="K10" s="7"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="9"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3"/>
@@ -918,13 +932,13 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="7"/>
       <c r="J11" s="3"/>
-      <c r="K11" s="8"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="9"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3"/>

</xml_diff>

<commit_message>
best model so far, 140/80 BP group, most distinct 3 groups using 10% subset
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Data Used</t>
   </si>
@@ -94,7 +94,7 @@
     <t>28012 x 1081</t>
   </si>
   <si>
-    <t>&gt; 160/80</t>
+    <t>&gt; 160/100</t>
   </si>
   <si>
     <t>age, sex</t>
@@ -121,7 +121,7 @@
     <t>82.4 &amp; 71.7</t>
   </si>
   <si>
-    <t>2802 x 1081</t>
+    <t>2801 x 1081</t>
   </si>
   <si>
     <t>62.4 &amp; 42.8</t>
@@ -137,6 +137,12 @@
   </si>
   <si>
     <t>17.3 &amp; 9.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -378 &amp; -40.7</t>
+  </si>
+  <si>
+    <t>8.6 &amp; 7.1</t>
   </si>
 </sst>
 </file>
@@ -873,21 +879,49 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="7"/>
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="5">
+        <v>50</v>
+      </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="8"/>
+      <c r="K8" s="5">
+        <v>440</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="5">
+        <v>17</v>
+      </c>
+      <c r="O8" s="6">
+        <v>47.5</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3"/>

</xml_diff>

<commit_message>
re-compiled matlab script, test different matlab parameters and finalize matlab script
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
   <si>
     <t>Data Used</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Row Subset</t>
   </si>
   <si>
-    <t>Target Definition</t>
+    <t>Target</t>
   </si>
   <si>
     <t>Normalize</t>
@@ -67,7 +67,7 @@
     <t>all</t>
   </si>
   <si>
-    <t>no event</t>
+    <t>no events</t>
   </si>
   <si>
     <t>&gt; 140/80</t>
@@ -143,6 +143,30 @@
   </si>
   <si>
     <t>8.6 &amp; 7.1</t>
+  </si>
+  <si>
+    <t>2884 x 1081</t>
+  </si>
+  <si>
+    <t>-142 &amp; -22.2</t>
+  </si>
+  <si>
+    <t>26.4 &amp; 27.5</t>
+  </si>
+  <si>
+    <t>-71.3 &amp; 23.8</t>
+  </si>
+  <si>
+    <t>43.8 &amp; 37.3</t>
+  </si>
+  <si>
+    <t>-379 &amp; -40.7</t>
+  </si>
+  <si>
+    <t>-183 &amp; -31.1</t>
+  </si>
+  <si>
+    <t>19.4 &amp; 15.4</t>
   </si>
 </sst>
 </file>
@@ -150,7 +174,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,12 +192,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -225,10 +243,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -542,7 +560,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -551,8 +569,8 @@
     <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
@@ -878,7 +896,7 @@
         <v>68.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -923,73 +941,219 @@
         <v>47.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="7"/>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="5">
+        <v>50</v>
+      </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="7"/>
+      <c r="K9" s="5">
+        <v>439</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N9" s="5">
+        <v>17</v>
+      </c>
+      <c r="O9" s="6">
+        <v>43.3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="5">
+        <v>10</v>
+      </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="7"/>
+      <c r="K10" s="5">
+        <v>405</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="5">
+        <v>8</v>
+      </c>
+      <c r="O10" s="6">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I11" s="5">
+        <v>50</v>
+      </c>
       <c r="J11" s="3"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="5"/>
+      <c r="K11" s="5">
+        <v>440</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="5">
+        <v>16</v>
+      </c>
+      <c r="O11" s="6">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+      <c r="A12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="5">
+        <v>50</v>
+      </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="K12" s="7">
+        <v>454</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="N12" s="7">
+        <v>16</v>
+      </c>
+      <c r="O12" s="8">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more job runs (full dataset run + very small dataset run)
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="56">
   <si>
     <t>Data Used</t>
   </si>
@@ -94,12 +94,18 @@
     <t>28012 x 1081</t>
   </si>
   <si>
+    <t>age, sex</t>
+  </si>
+  <si>
+    <t>87.5 &amp; 81.4</t>
+  </si>
+  <si>
+    <t>84.2 &amp; 74.2</t>
+  </si>
+  <si>
     <t>&gt; 160/100</t>
   </si>
   <si>
-    <t>age, sex</t>
-  </si>
-  <si>
     <t>94.0 &amp; 81.9</t>
   </si>
   <si>
@@ -167,6 +173,15 @@
   </si>
   <si>
     <t>19.4 &amp; 15.4</t>
+  </si>
+  <si>
+    <t>1401 x 1081</t>
+  </si>
+  <si>
+    <t>-52.9 &amp; -3.6</t>
+  </si>
+  <si>
+    <t>15.9 &amp; 17.1</t>
   </si>
 </sst>
 </file>
@@ -223,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -241,12 +256,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -560,27 +569,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -685,7 +694,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>19</v>
@@ -694,23 +703,23 @@
         <v>20</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I3" s="5">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="5">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="L3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="N3" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O3" s="6">
         <v>47.5</v>
@@ -730,35 +739,35 @@
         <v>17</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="5">
         <v>25</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="5">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="L4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="N4" s="5">
         <v>17</v>
       </c>
       <c r="O4" s="6">
-        <v>11.8</v>
+        <v>47.5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -775,23 +784,23 @@
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I5" s="5">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="5">
-        <v>55</v>
+        <v>105</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>33</v>
@@ -800,10 +809,10 @@
         <v>34</v>
       </c>
       <c r="N5" s="5">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="O5" s="6">
-        <v>75.6</v>
+        <v>11.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -811,7 +820,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>16</v>
@@ -820,7 +829,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>19</v>
@@ -829,26 +838,26 @@
         <v>20</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I6" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="5">
-        <v>429</v>
+        <v>55</v>
       </c>
       <c r="L6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="M6" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="N6" s="5">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="O6" s="6">
-        <v>57.2</v>
+        <v>75.6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -856,7 +865,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -865,7 +874,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -874,26 +883,26 @@
         <v>20</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I7" s="5">
         <v>50</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="5">
-        <v>260</v>
+        <v>429</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="N7" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O7" s="6">
-        <v>68.9</v>
+        <v>57.2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -901,7 +910,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
@@ -910,7 +919,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
@@ -919,14 +928,14 @@
         <v>20</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I8" s="5">
         <v>50</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="5">
-        <v>440</v>
+        <v>260</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>41</v>
@@ -935,10 +944,10 @@
         <v>42</v>
       </c>
       <c r="N8" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O8" s="6">
-        <v>47.5</v>
+        <v>68.9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -946,13 +955,13 @@
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
@@ -964,26 +973,26 @@
         <v>20</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="5">
         <v>50</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="5">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="L9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="N9" s="5">
         <v>17</v>
       </c>
       <c r="O9" s="6">
-        <v>43.3</v>
+        <v>47.5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -991,13 +1000,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
@@ -1009,14 +1018,14 @@
         <v>20</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5">
-        <v>405</v>
+        <v>439</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>46</v>
@@ -1025,10 +1034,10 @@
         <v>47</v>
       </c>
       <c r="N10" s="5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="O10" s="6">
-        <v>9.8</v>
+        <v>43.3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -1036,7 +1045,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>
@@ -1051,37 +1060,37 @@
         <v>19</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I11" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="5">
-        <v>440</v>
+        <v>405</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>48</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="N11" s="5">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="O11" s="6">
-        <v>24.8</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <v>9.8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>16</v>
@@ -1096,64 +1105,171 @@
         <v>19</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I12" s="5">
         <v>50</v>
       </c>
       <c r="J12" s="3"/>
-      <c r="K12" s="7">
+      <c r="K12" s="5">
+        <v>440</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="5">
+        <v>16</v>
+      </c>
+      <c r="O12" s="6">
+        <v>24.8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="5">
+        <v>50</v>
+      </c>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5">
         <v>454</v>
       </c>
-      <c r="L12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="M12" s="3" t="s">
+      <c r="L13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N13" s="5">
+        <v>16</v>
+      </c>
+      <c r="O13" s="6">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="5">
         <v>50</v>
       </c>
-      <c r="N12" s="7">
-        <v>16</v>
-      </c>
-      <c r="O12" s="8">
-        <v>27.2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="5"/>
       <c r="J14" s="3"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="6"/>
+      <c r="K14" s="5">
+        <v>437</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N14" s="5">
+        <v>16</v>
+      </c>
+      <c r="O14" s="6">
+        <v>32.7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated job history with new (but unsuccessful) run of full dataset without Event column
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
   <si>
     <t>Data Used</t>
   </si>
@@ -127,6 +127,12 @@
     <t>82.4 &amp; 71.7</t>
   </si>
   <si>
+    <t>89.7 &amp; 83.3</t>
+  </si>
+  <si>
+    <t>81.6 &amp; 70.3</t>
+  </si>
+  <si>
     <t>2801 x 1081</t>
   </si>
   <si>
@@ -182,6 +188,9 @@
   </si>
   <si>
     <t>15.9 &amp; 17.1</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -238,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -257,6 +266,9 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -569,27 +581,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -860,12 +872,12 @@
         <v>75.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>16</v>
@@ -874,7 +886,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>19</v>
@@ -890,19 +902,19 @@
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="5">
-        <v>429</v>
+        <v>87</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="N7" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="O7" s="6">
-        <v>57.2</v>
+        <v>47.5081</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -910,7 +922,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
@@ -935,19 +947,19 @@
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="5">
-        <v>260</v>
+        <v>429</v>
       </c>
       <c r="L8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="N8" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="O8" s="6">
-        <v>68.9</v>
+        <v>57.2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -955,7 +967,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>16</v>
@@ -964,7 +976,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>19</v>
@@ -980,7 +992,7 @@
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="5">
-        <v>440</v>
+        <v>260</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>43</v>
@@ -989,10 +1001,10 @@
         <v>44</v>
       </c>
       <c r="N9" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O9" s="6">
-        <v>47.5</v>
+        <v>68.9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -1000,13 +1012,13 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>18</v>
@@ -1025,19 +1037,19 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="L10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="N10" s="5">
         <v>17</v>
       </c>
       <c r="O10" s="6">
-        <v>43.3</v>
+        <v>47.5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -1045,13 +1057,13 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>18</v>
@@ -1066,11 +1078,11 @@
         <v>26</v>
       </c>
       <c r="I11" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="5">
-        <v>405</v>
+        <v>439</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>48</v>
@@ -1079,10 +1091,10 @@
         <v>49</v>
       </c>
       <c r="N11" s="5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="O11" s="6">
-        <v>9.8</v>
+        <v>43.3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -1090,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>16</v>
@@ -1105,29 +1117,29 @@
         <v>19</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I12" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="5">
-        <v>440</v>
+        <v>405</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>50</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="N12" s="5">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="O12" s="6">
-        <v>24.8</v>
+        <v>9.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1135,7 +1147,7 @@
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>16</v>
@@ -1150,29 +1162,29 @@
         <v>19</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I13" s="5">
         <v>50</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="5">
-        <v>454</v>
+        <v>440</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N13" s="5">
         <v>16</v>
       </c>
       <c r="O13" s="6">
-        <v>27.2</v>
+        <v>24.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1180,7 +1192,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
@@ -1205,47 +1217,91 @@
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="5">
+        <v>454</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N14" s="5">
+        <v>16</v>
+      </c>
+      <c r="O14" s="6">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="5">
+        <v>50</v>
+      </c>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5">
         <v>437</v>
       </c>
-      <c r="L14" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="N14" s="5">
-        <v>16</v>
-      </c>
-      <c r="O14" s="6">
+      <c r="L15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="N15" s="5">
+        <v>16</v>
+      </c>
+      <c r="O15" s="6">
         <v>32.7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
-    </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="A16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="I16" s="5"/>
       <c r="J16" s="3"/>
       <c r="K16" s="5"/>
@@ -1271,6 +1327,23 @@
       <c r="N17" s="5"/>
       <c r="O17" s="6"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ran whole dataset with subset of most overlapping variables
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="61">
   <si>
     <t>Data Used</t>
   </si>
@@ -190,7 +190,13 @@
     <t>15.9 &amp; 17.1</t>
   </si>
   <si>
-    <t/>
+    <t>28012 x 566</t>
+  </si>
+  <si>
+    <t>96.2 &amp; 88.8</t>
+  </si>
+  <si>
+    <t>76.7 &amp; 67.2</t>
   </si>
 </sst>
 </file>
@@ -247,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -266,9 +272,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -587,21 +590,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -872,7 +875,7 @@
         <v>75.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1278,37 +1281,49 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I16" s="5"/>
+      <c r="C16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I16" s="5">
+        <v>50</v>
+      </c>
       <c r="J16" s="3"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
+      <c r="K16" s="5">
+        <v>63</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N16" s="5">
+        <v>18</v>
+      </c>
+      <c r="O16" s="6">
+        <v>11.77</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3"/>

</xml_diff>

<commit_message>
ran new job with less variables, moved mean up but seperation of groups unclear
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="64">
   <si>
     <t>Data Used</t>
   </si>
@@ -197,6 +197,15 @@
   </si>
   <si>
     <t>76.7 &amp; 67.2</t>
+  </si>
+  <si>
+    <t>28012 x 145</t>
+  </si>
+  <si>
+    <t>100.3 &amp; 101.3</t>
+  </si>
+  <si>
+    <t>85.0 &amp; 84.3</t>
   </si>
 </sst>
 </file>
@@ -253,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -271,6 +280,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -584,27 +599,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1326,23 +1341,51 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="5"/>
+      <c r="A17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="5">
+        <v>50</v>
+      </c>
       <c r="J17" s="3"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="K17" s="5">
+        <v>37</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N17" s="5">
+        <v>17</v>
+      </c>
+      <c r="O17" s="6">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1351,13 +1394,81 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="5"/>
+      <c r="I18" s="7"/>
       <c r="J18" s="3"/>
-      <c r="K18" s="5"/>
+      <c r="K18" s="7"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
re-ran 10% of dataset with more concentrated variables, this actually made it worse
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="68">
   <si>
     <t>Data Used</t>
   </si>
@@ -133,6 +133,24 @@
     <t>81.6 &amp; 70.3</t>
   </si>
   <si>
+    <t>28012 x 566</t>
+  </si>
+  <si>
+    <t>96.2 &amp; 88.8</t>
+  </si>
+  <si>
+    <t>76.7 &amp; 67.2</t>
+  </si>
+  <si>
+    <t>28012 x 145</t>
+  </si>
+  <si>
+    <t>100.3 &amp; 101.3</t>
+  </si>
+  <si>
+    <t>85.0 &amp; 84.3</t>
+  </si>
+  <si>
     <t>2801 x 1081</t>
   </si>
   <si>
@@ -190,22 +208,16 @@
     <t>15.9 &amp; 17.1</t>
   </si>
   <si>
-    <t>28012 x 566</t>
-  </si>
-  <si>
-    <t>96.2 &amp; 88.8</t>
-  </si>
-  <si>
-    <t>76.7 &amp; 67.2</t>
-  </si>
-  <si>
-    <t>28012 x 145</t>
-  </si>
-  <si>
-    <t>100.3 &amp; 101.3</t>
-  </si>
-  <si>
-    <t>85.0 &amp; 84.3</t>
+    <t>2801 x 145</t>
+  </si>
+  <si>
+    <t>86.1 &amp; 85.7</t>
+  </si>
+  <si>
+    <t>55.9 &amp; 42.1</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -213,7 +225,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +243,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -262,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -282,11 +300,14 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -599,27 +620,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="14.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="14.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="12" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -935,7 +956,7 @@
         <v>47.5081</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -949,7 +970,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>19</v>
@@ -958,14 +979,14 @@
         <v>20</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I8" s="5">
         <v>50</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="5">
-        <v>429</v>
+        <v>63</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>40</v>
@@ -974,13 +995,13 @@
         <v>41</v>
       </c>
       <c r="N8" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="O8" s="6">
-        <v>57.2</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+        <v>11.77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -994,7 +1015,7 @@
         <v>17</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>19</v>
@@ -1003,14 +1024,14 @@
         <v>20</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="I9" s="5">
         <v>50</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="5">
-        <v>260</v>
+        <v>37</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>43</v>
@@ -1019,10 +1040,10 @@
         <v>44</v>
       </c>
       <c r="N9" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O9" s="6">
-        <v>68.9</v>
+        <v>3.51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -1030,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>16</v>
@@ -1039,7 +1060,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>19</v>
@@ -1055,19 +1076,19 @@
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="5">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N10" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" s="6">
-        <v>47.5</v>
+        <v>57.2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -1075,16 +1096,16 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>19</v>
@@ -1100,19 +1121,19 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="5">
-        <v>439</v>
+        <v>260</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N11" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O11" s="6">
-        <v>43.3</v>
+        <v>68.9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -1120,7 +1141,7 @@
         <v>24</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>16</v>
@@ -1141,23 +1162,23 @@
         <v>26</v>
       </c>
       <c r="I12" s="5">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="5">
-        <v>405</v>
+        <v>440</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N12" s="5">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="O12" s="6">
-        <v>9.8</v>
+        <v>47.5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1165,13 +1186,13 @@
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>18</v>
@@ -1180,7 +1201,7 @@
         <v>19</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>26</v>
@@ -1190,19 +1211,19 @@
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="5">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="N13" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O13" s="6">
-        <v>24.8</v>
+        <v>43.3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1210,7 +1231,7 @@
         <v>24</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>16</v>
@@ -1228,26 +1249,26 @@
         <v>20</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I14" s="5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="5">
-        <v>454</v>
+        <v>405</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="N14" s="5">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="O14" s="6">
-        <v>27.2</v>
+        <v>9.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1255,7 +1276,7 @@
         <v>24</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>16</v>
@@ -1270,29 +1291,29 @@
         <v>19</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I15" s="5">
         <v>50</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="5">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="N15" s="5">
         <v>16</v>
       </c>
       <c r="O15" s="6">
-        <v>32.7</v>
+        <v>24.8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -1300,7 +1321,7 @@
         <v>24</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>16</v>
@@ -1325,7 +1346,7 @@
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="5">
-        <v>63</v>
+        <v>454</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>59</v>
@@ -1334,10 +1355,10 @@
         <v>60</v>
       </c>
       <c r="N16" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="O16" s="6">
-        <v>11.77</v>
+        <v>27.2</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
@@ -1370,7 +1391,7 @@
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="5">
-        <v>37</v>
+        <v>437</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>62</v>
@@ -1379,60 +1400,128 @@
         <v>63</v>
       </c>
       <c r="N17" s="5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O17" s="6">
-        <v>3.51</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="7"/>
+        <v>32.7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" s="5">
+        <v>50</v>
+      </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="7"/>
+      <c r="K18" s="7">
+        <v>51</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="N18" s="7">
+        <v>18</v>
+      </c>
+      <c r="O18" s="8">
+        <v>4.23</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I19" s="5"/>
       <c r="J19" s="3"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="8"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N19" s="5"/>
+      <c r="O19" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="7"/>
+      <c r="A20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="5"/>
       <c r="J20" s="3"/>
       <c r="K20" s="7"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M20" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="N20" s="7"/>
       <c r="O20" s="8"/>
     </row>
@@ -1453,7 +1542,7 @@
       <c r="N21" s="7"/>
       <c r="O21" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1462,13 +1551,47 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="7"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="5"/>
+      <c r="K22" s="7"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="6"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran entire dataset on BP vars only
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="72">
   <si>
     <t>Data Used</t>
   </si>
@@ -220,7 +220,16 @@
     <t>55.9 &amp; 42.1</t>
   </si>
   <si>
-    <t/>
+    <t>28012 x 4</t>
+  </si>
+  <si>
+    <t>Sex/Age/BP only</t>
+  </si>
+  <si>
+    <t>47.7 &amp; 35.8</t>
+  </si>
+  <si>
+    <t>19.9 &amp; 43.8</t>
   </si>
 </sst>
 </file>
@@ -228,7 +237,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,12 +255,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -283,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -302,15 +305,6 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -629,21 +623,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="10" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="10" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="10" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="10" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="10" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="11" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="10" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="10" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="11" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="12" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -959,7 +953,7 @@
         <v>47.5081</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -1004,7 +998,7 @@
         <v>11.77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -1438,7 +1432,7 @@
         <v>50</v>
       </c>
       <c r="J18" s="3"/>
-      <c r="K18" s="7">
+      <c r="K18" s="5">
         <v>51</v>
       </c>
       <c r="L18" s="3" t="s">
@@ -1447,88 +1441,76 @@
       <c r="M18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="N18" s="7">
-        <v>18</v>
-      </c>
-      <c r="O18" s="8">
+      <c r="N18" s="5">
+        <v>18</v>
+      </c>
+      <c r="O18" s="6">
         <v>4.23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I19" s="5"/>
+      <c r="C19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="5">
+        <v>50</v>
+      </c>
       <c r="J19" s="3"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="M19" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>68</v>
-      </c>
+      <c r="K19" s="5">
+        <v>3</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="N19" s="5">
+        <v>3</v>
+      </c>
+      <c r="O19" s="6">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
       <c r="I20" s="5"/>
       <c r="J20" s="3"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="N20" s="7"/>
-      <c r="O20" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+      <c r="K20" s="5"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1537,15 +1519,15 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="7"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="3"/>
-      <c r="K21" s="7"/>
+      <c r="K21" s="5"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+      <c r="N21" s="5"/>
+      <c r="O21" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1554,15 +1536,15 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="7"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="3"/>
-      <c r="K22" s="7"/>
+      <c r="K22" s="5"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="N22" s="5"/>
+      <c r="O22" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1571,13 +1553,13 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="7"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="3"/>
-      <c r="K23" s="7"/>
+      <c r="K23" s="5"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="8"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3"/>

</xml_diff>

<commit_message>
job outputs for subsets of datasets 50% 25% 10% for only BP/Sex/Age
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
   <si>
     <t>Data Used</t>
   </si>
@@ -230,6 +230,33 @@
   </si>
   <si>
     <t>19.9 &amp; 43.8</t>
+  </si>
+  <si>
+    <t>14006 x 4</t>
+  </si>
+  <si>
+    <t>50.2 &amp; 16.6</t>
+  </si>
+  <si>
+    <t>33.1 &amp; 78.8</t>
+  </si>
+  <si>
+    <t>7003 x 4</t>
+  </si>
+  <si>
+    <t>60.4 &amp; 28.0</t>
+  </si>
+  <si>
+    <t>82.1 &amp; 119.2</t>
+  </si>
+  <si>
+    <t>2801 x 4</t>
+  </si>
+  <si>
+    <t>83.5 &amp; 106.7</t>
+  </si>
+  <si>
+    <t>53.6 &amp; 132.2</t>
   </si>
 </sst>
 </file>
@@ -1494,55 +1521,139 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="5"/>
+      <c r="A20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="5">
+        <v>50</v>
+      </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="6"/>
+      <c r="K20" s="5">
+        <v>3</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="M20" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="N20" s="5">
+        <v>3</v>
+      </c>
+      <c r="O20" s="6">
+        <v>1.18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="5"/>
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="5">
+        <v>50</v>
+      </c>
       <c r="J21" s="3"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="3"/>
-      <c r="M21" s="3"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="6"/>
+      <c r="K21" s="5">
+        <v>2</v>
+      </c>
+      <c r="L21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="N21" s="5">
+        <v>3</v>
+      </c>
+      <c r="O21" s="6">
+        <v>0.31</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="5"/>
+      <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" s="5">
+        <v>50</v>
+      </c>
       <c r="J22" s="3"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="6"/>
+      <c r="K22" s="5">
+        <v>3</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N22" s="5">
+        <v>3</v>
+      </c>
+      <c r="O22" s="6">
+        <v>1.02</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3"/>

</xml_diff>

<commit_message>
produce runs with only BP variable, with 10% 25% 50% and 100% of dataset
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="94">
   <si>
     <t>Data Used</t>
   </si>
@@ -257,6 +257,45 @@
   </si>
   <si>
     <t>53.6 &amp; 132.2</t>
+  </si>
+  <si>
+    <t>28012 x 2</t>
+  </si>
+  <si>
+    <t>BP only</t>
+  </si>
+  <si>
+    <t>6.4 &amp; 2.2</t>
+  </si>
+  <si>
+    <t>19.8 &amp; 52.4</t>
+  </si>
+  <si>
+    <t>14006 x 2</t>
+  </si>
+  <si>
+    <t>-3.6 &amp; -0.7</t>
+  </si>
+  <si>
+    <t>34.8 &amp; -0.7</t>
+  </si>
+  <si>
+    <t>7003 x 2</t>
+  </si>
+  <si>
+    <t>-39.9 &amp; -9.9</t>
+  </si>
+  <si>
+    <t>35.5 &amp; 133.9</t>
+  </si>
+  <si>
+    <t>2801 x 2</t>
+  </si>
+  <si>
+    <t>51.9 &amp; 15.5</t>
+  </si>
+  <si>
+    <t>28.3 &amp; 79.9</t>
   </si>
 </sst>
 </file>
@@ -313,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -331,6 +370,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -644,27 +689,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1655,39 +1700,219 @@
         <v>1.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="5"/>
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="5">
+        <v>50</v>
+      </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="5"/>
+      <c r="K23" s="7">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="N23" s="7">
+        <v>2</v>
+      </c>
+      <c r="O23" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+      <c r="A24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="5">
+        <v>50</v>
+      </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="6"/>
+      <c r="K24" s="7">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N24" s="7">
+        <v>2</v>
+      </c>
+      <c r="O24" s="8">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+      <c r="A25" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="5">
+        <v>50</v>
+      </c>
+      <c r="J25" s="3"/>
+      <c r="K25" s="7">
+        <v>1</v>
+      </c>
+      <c r="L25" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="N25" s="7">
+        <v>2</v>
+      </c>
+      <c r="O25" s="8">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+      <c r="A26" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I26" s="5">
+        <v>50</v>
+      </c>
+      <c r="J26" s="3"/>
+      <c r="K26" s="7">
+        <v>1</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="N26" s="7">
+        <v>2</v>
+      </c>
+      <c r="O26" s="8">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran whole dataset will all columns with 160/100 target definition
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="96">
   <si>
     <t>Data Used</t>
   </si>
@@ -296,6 +296,12 @@
   </si>
   <si>
     <t>28.3 &amp; 79.9</t>
+  </si>
+  <si>
+    <t>95.7 &amp; 81.1</t>
+  </si>
+  <si>
+    <t>72.2 &amp; 57.6</t>
   </si>
 </sst>
 </file>
@@ -303,7 +309,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -321,6 +327,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -352,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -370,6 +382,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -689,27 +707,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="12" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="13" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1700,7 +1718,7 @@
         <v>1.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
         <v>24</v>
       </c>
@@ -1745,7 +1763,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
         <v>24</v>
       </c>
@@ -1790,7 +1808,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1880,24 +1898,52 @@
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="5"/>
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+      <c r="A27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I27" s="5">
+        <v>50</v>
+      </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+      <c r="K27" s="9">
+        <v>102</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="N27" s="9">
+        <v>19</v>
+      </c>
+      <c r="O27" s="10">
+        <v>52.1</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1906,13 +1952,81 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="5"/>
+      <c r="I28" s="9"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="5"/>
+      <c r="K28" s="9"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="6"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
removed rows with outlier disease scores, made final distribution slightly better but groups still not separated clearly
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="100">
   <si>
     <t>Data Used</t>
   </si>
@@ -302,6 +302,18 @@
   </si>
   <si>
     <t>72.2 &amp; 57.6</t>
+  </si>
+  <si>
+    <t>26474 x 1081</t>
+  </si>
+  <si>
+    <t>no events, remove outliers</t>
+  </si>
+  <si>
+    <t>91.7 &amp; 90.4</t>
+  </si>
+  <si>
+    <t>79.5 &amp; 75.2</t>
   </si>
 </sst>
 </file>
@@ -707,7 +719,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -716,7 +728,7 @@
     <col min="1" max="1" style="11" width="20.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="11" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="11" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="23.290714285714284" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
@@ -1747,7 +1759,7 @@
         <v>50</v>
       </c>
       <c r="J23" s="3"/>
-      <c r="K23" s="7">
+      <c r="K23" s="5">
         <v>1</v>
       </c>
       <c r="L23" s="3" t="s">
@@ -1756,10 +1768,10 @@
       <c r="M23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="N23" s="7">
+      <c r="N23" s="5">
         <v>2</v>
       </c>
-      <c r="O23" s="8">
+      <c r="O23" s="6">
         <v>1.5</v>
       </c>
     </row>
@@ -1792,7 +1804,7 @@
         <v>50</v>
       </c>
       <c r="J24" s="3"/>
-      <c r="K24" s="7">
+      <c r="K24" s="5">
         <v>1</v>
       </c>
       <c r="L24" s="3" t="s">
@@ -1801,10 +1813,10 @@
       <c r="M24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="N24" s="7">
+      <c r="N24" s="5">
         <v>2</v>
       </c>
-      <c r="O24" s="8">
+      <c r="O24" s="6">
         <v>1.45</v>
       </c>
     </row>
@@ -1837,7 +1849,7 @@
         <v>50</v>
       </c>
       <c r="J25" s="3"/>
-      <c r="K25" s="7">
+      <c r="K25" s="5">
         <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
@@ -1846,14 +1858,14 @@
       <c r="M25" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N25" s="7">
+      <c r="N25" s="5">
         <v>2</v>
       </c>
-      <c r="O25" s="8">
+      <c r="O25" s="6">
         <v>1.3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -1882,7 +1894,7 @@
         <v>50</v>
       </c>
       <c r="J26" s="3"/>
-      <c r="K26" s="7">
+      <c r="K26" s="5">
         <v>1</v>
       </c>
       <c r="L26" s="3" t="s">
@@ -1891,14 +1903,14 @@
       <c r="M26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="N26" s="7">
+      <c r="N26" s="5">
         <v>2</v>
       </c>
-      <c r="O26" s="8">
+      <c r="O26" s="6">
         <v>0.01</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3" t="s">
         <v>24</v>
       </c>
@@ -1906,7 +1918,7 @@
         <v>25</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>17</v>
@@ -1927,7 +1939,7 @@
         <v>50</v>
       </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="9">
+      <c r="K27" s="7">
         <v>102</v>
       </c>
       <c r="L27" s="3" t="s">
@@ -1936,29 +1948,57 @@
       <c r="M27" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N27" s="9">
-        <v>19</v>
-      </c>
-      <c r="O27" s="10">
+      <c r="N27" s="7">
+        <v>19</v>
+      </c>
+      <c r="O27" s="8">
         <v>52.1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="9"/>
+      <c r="A28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I28" s="5">
+        <v>50</v>
+      </c>
       <c r="J28" s="3"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="10"/>
+      <c r="K28" s="7">
+        <v>85</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="N28" s="7">
+        <v>18</v>
+      </c>
+      <c r="O28" s="8">
+        <v>15.6</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3"/>
@@ -1986,15 +2026,15 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="9"/>
+      <c r="I30" s="7"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="9"/>
+      <c r="K30" s="7"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="N30" s="7"/>
+      <c r="O30" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -2003,13 +2043,13 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="5"/>
+      <c r="I31" s="7"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="5"/>
+      <c r="K31" s="7"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="6"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3"/>
@@ -2028,6 +2068,23 @@
       <c r="N32" s="5"/>
       <c r="O32" s="6"/>
     </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
run 10% subset with less columns, results are also not good
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="102">
   <si>
     <t>Data Used</t>
   </si>
@@ -314,6 +314,12 @@
   </si>
   <si>
     <t>79.5 &amp; 75.2</t>
+  </si>
+  <si>
+    <t>93.1 &amp; 82.5</t>
+  </si>
+  <si>
+    <t>52.1 &amp; 51.4</t>
   </si>
 </sst>
 </file>
@@ -376,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -400,12 +406,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -725,21 +725,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1939,7 +1939,7 @@
         <v>50</v>
       </c>
       <c r="J27" s="3"/>
-      <c r="K27" s="7">
+      <c r="K27" s="5">
         <v>102</v>
       </c>
       <c r="L27" s="3" t="s">
@@ -1948,14 +1948,14 @@
       <c r="M27" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="N27" s="7">
-        <v>19</v>
-      </c>
-      <c r="O27" s="8">
+      <c r="N27" s="5">
+        <v>19</v>
+      </c>
+      <c r="O27" s="6">
         <v>52.1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>50</v>
       </c>
       <c r="J28" s="3"/>
-      <c r="K28" s="7">
+      <c r="K28" s="5">
         <v>85</v>
       </c>
       <c r="L28" s="3" t="s">
@@ -1993,29 +1993,57 @@
       <c r="M28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="N28" s="7">
-        <v>18</v>
-      </c>
-      <c r="O28" s="8">
+      <c r="N28" s="5">
+        <v>18</v>
+      </c>
+      <c r="O28" s="6">
         <v>15.6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="9"/>
+      <c r="A29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I29" s="5">
+        <v>50</v>
+      </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="10"/>
+      <c r="K29" s="7">
+        <v>51</v>
+      </c>
+      <c r="L29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="N29" s="7">
+        <v>17</v>
+      </c>
+      <c r="O29" s="8">
+        <v>2.66</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3"/>
@@ -2026,13 +2054,13 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="7"/>
+      <c r="I30" s="5"/>
       <c r="J30" s="3"/>
-      <c r="K30" s="7"/>
+      <c r="K30" s="5"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
-      <c r="N30" s="7"/>
-      <c r="O30" s="8"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3"/>
@@ -2043,13 +2071,13 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="7"/>
+      <c r="I31" s="5"/>
       <c r="J31" s="3"/>
-      <c r="K31" s="7"/>
+      <c r="K31" s="5"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
-      <c r="N31" s="7"/>
-      <c r="O31" s="8"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3"/>

</xml_diff>

<commit_message>
re-ran 10% subset with only most weighted variables but the results were worsed...
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="106">
   <si>
     <t>Data Used</t>
   </si>
@@ -320,6 +320,18 @@
   </si>
   <si>
     <t>52.1 &amp; 51.4</t>
+  </si>
+  <si>
+    <t>2801 x 462</t>
+  </si>
+  <si>
+    <t>subrun fts</t>
+  </si>
+  <si>
+    <t>-230.9 &amp; -42.0</t>
+  </si>
+  <si>
+    <t>45.8 &amp; 40.4</t>
   </si>
 </sst>
 </file>
@@ -327,7 +339,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,12 +357,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -382,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -400,12 +406,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -725,21 +725,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="11.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2000,7 +2000,7 @@
         <v>15.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3" t="s">
         <v>24</v>
       </c>
@@ -2029,7 +2029,7 @@
         <v>50</v>
       </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="7">
+      <c r="K29" s="5">
         <v>51</v>
       </c>
       <c r="L29" s="3" t="s">
@@ -2038,29 +2038,57 @@
       <c r="M29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="N29" s="7">
-        <v>17</v>
-      </c>
-      <c r="O29" s="8">
+      <c r="N29" s="5">
+        <v>17</v>
+      </c>
+      <c r="O29" s="6">
         <v>2.66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="5"/>
+      <c r="A30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I30" s="5">
+        <v>50</v>
+      </c>
       <c r="J30" s="3"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="6"/>
+      <c r="K30" s="5">
+        <v>114</v>
+      </c>
+      <c r="L30" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="N30" s="5">
+        <v>19</v>
+      </c>
+      <c r="O30" s="6">
+        <v>68.9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3"/>

</xml_diff>

<commit_message>
ran full run with subset obtained from 10% subrun most weighted variables, results show that the mean was moved up but the seperation of variables are still not that big
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="109">
   <si>
     <t>Data Used</t>
   </si>
@@ -332,6 +332,15 @@
   </si>
   <si>
     <t>45.8 &amp; 40.4</t>
+  </si>
+  <si>
+    <t>28012 x 462</t>
+  </si>
+  <si>
+    <t>100.8 &amp; 94.2</t>
+  </si>
+  <si>
+    <t>78.0 &amp; 70.9</t>
   </si>
 </sst>
 </file>
@@ -388,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -406,6 +415,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -719,27 +734,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2045,7 +2060,7 @@
         <v>2.66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
@@ -2090,24 +2105,52 @@
         <v>68.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="5"/>
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+      <c r="A31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I31" s="5">
+        <v>50</v>
+      </c>
       <c r="J31" s="3"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+      <c r="K31" s="5">
+        <v>54</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="M31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="N31" s="5">
+        <v>18</v>
+      </c>
+      <c r="O31" s="6">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2116,15 +2159,15 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="5"/>
+      <c r="I32" s="7"/>
       <c r="J32" s="3"/>
-      <c r="K32" s="5"/>
+      <c r="K32" s="7"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="N32" s="7"/>
+      <c r="O32" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2133,13 +2176,132 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="7"/>
       <c r="J33" s="3"/>
-      <c r="K33" s="5"/>
+      <c r="K33" s="7"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="6"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="5"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
obtained distance matrix for 25% subset run
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
   <si>
     <t>Data Used</t>
   </si>
@@ -341,6 +341,15 @@
   </si>
   <si>
     <t>78.0 &amp; 70.9</t>
+  </si>
+  <si>
+    <t>7003 x 1084</t>
+  </si>
+  <si>
+    <t>-117.4 &amp; -29.7</t>
+  </si>
+  <si>
+    <t>49.4 &amp; 33.8</t>
   </si>
 </sst>
 </file>
@@ -348,7 +357,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +375,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -417,10 +432,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -751,7 +766,7 @@
     <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
     <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
@@ -2151,21 +2166,49 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="7"/>
+      <c r="A32" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I32" s="5">
+        <v>50</v>
+      </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="8"/>
+      <c r="K32" s="7">
+        <v>243</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M32" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="N32" s="7">
+        <v>16</v>
+      </c>
+      <c r="O32" s="8">
+        <v>68.9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3"/>

</xml_diff>

<commit_message>
ran most refined subsets to investigate distance matrices, seems that there is definetly a trend
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="116">
   <si>
     <t>Data Used</t>
   </si>
   <si>
-    <t>Subset Dimensions</t>
+    <t>Subset Dim</t>
   </si>
   <si>
     <t>Column Subset</t>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>49.4 &amp; 33.8</t>
+  </si>
+  <si>
+    <t>4092 x 1081</t>
+  </si>
+  <si>
+    <t>-503.9 &amp; -60.4</t>
+  </si>
+  <si>
+    <t>44.2 &amp; 32.8</t>
+  </si>
+  <si>
+    <t>9328 x 1081</t>
   </si>
 </sst>
 </file>
@@ -357,7 +369,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,12 +387,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -412,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -430,12 +436,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -755,21 +755,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="20.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2165,7 +2165,7 @@
         <v>12.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3" t="s">
         <v>24</v>
       </c>
@@ -2194,7 +2194,7 @@
         <v>50</v>
       </c>
       <c r="J32" s="3"/>
-      <c r="K32" s="7">
+      <c r="K32" s="5">
         <v>243</v>
       </c>
       <c r="L32" s="3" t="s">
@@ -2203,48 +2203,94 @@
       <c r="M32" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="N32" s="7">
-        <v>16</v>
-      </c>
-      <c r="O32" s="8">
+      <c r="N32" s="5">
+        <v>16</v>
+      </c>
+      <c r="O32" s="6">
         <v>68.9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="7"/>
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+      <c r="A33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I33" s="5">
+        <v>50</v>
+      </c>
       <c r="J33" s="3"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="7"/>
-      <c r="O33" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="7"/>
+      <c r="K33" s="5">
+        <v>386</v>
+      </c>
+      <c r="L33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="N33" s="5">
+        <v>17</v>
+      </c>
+      <c r="O33" s="6">
+        <v>75.6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+      <c r="A34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I34" s="5">
+        <v>50</v>
+      </c>
       <c r="J34" s="3"/>
-      <c r="K34" s="7"/>
+      <c r="K34" s="5"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
-      <c r="N34" s="7"/>
-      <c r="O34" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+      <c r="N34" s="5"/>
+      <c r="O34" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2253,15 +2299,15 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="7"/>
+      <c r="I35" s="5"/>
       <c r="J35" s="3"/>
-      <c r="K35" s="7"/>
+      <c r="K35" s="5"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+      <c r="N35" s="5"/>
+      <c r="O35" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2270,15 +2316,15 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="7"/>
+      <c r="I36" s="5"/>
       <c r="J36" s="3"/>
-      <c r="K36" s="7"/>
+      <c r="K36" s="5"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
-      <c r="N36" s="7"/>
-      <c r="O36" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+      <c r="N36" s="5"/>
+      <c r="O36" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2287,15 +2333,15 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="7"/>
+      <c r="I37" s="5"/>
       <c r="J37" s="3"/>
-      <c r="K37" s="7"/>
+      <c r="K37" s="5"/>
       <c r="L37" s="3"/>
       <c r="M37" s="3"/>
-      <c r="N37" s="7"/>
-      <c r="O37" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+      <c r="N37" s="5"/>
+      <c r="O37" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2304,13 +2350,13 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="7"/>
+      <c r="I38" s="5"/>
       <c r="J38" s="3"/>
-      <c r="K38" s="7"/>
+      <c r="K38" s="5"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
-      <c r="N38" s="7"/>
-      <c r="O38" s="8"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="3"/>

</xml_diff>

<commit_message>
ran few more jobs at different subset intervals
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="130">
   <si>
     <t>Data Used</t>
   </si>
@@ -362,6 +362,48 @@
   </si>
   <si>
     <t>9328 x 1081</t>
+  </si>
+  <si>
+    <t>34.5 &amp; 21.4</t>
+  </si>
+  <si>
+    <t>58.8 &amp; 43.7</t>
+  </si>
+  <si>
+    <t>2801 x 147</t>
+  </si>
+  <si>
+    <t>81.6 &amp; 77.4</t>
+  </si>
+  <si>
+    <t>68.3 &amp; 63.7</t>
+  </si>
+  <si>
+    <t>7003 x 147</t>
+  </si>
+  <si>
+    <t>95.8 &amp; 94.2</t>
+  </si>
+  <si>
+    <t>79.9 &amp; 75.2</t>
+  </si>
+  <si>
+    <t>4902 x 462</t>
+  </si>
+  <si>
+    <t>55.0 &amp; 40.7</t>
+  </si>
+  <si>
+    <t>48.9 &amp; 43.1</t>
+  </si>
+  <si>
+    <t>3502 x 1081</t>
+  </si>
+  <si>
+    <t>-398.3 &amp; -40.7</t>
+  </si>
+  <si>
+    <t>35.3 &amp; 34.9</t>
   </si>
 </sst>
 </file>
@@ -2038,7 +2080,7 @@
         <v>65</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>17</v>
@@ -2284,79 +2326,201 @@
         <v>50</v>
       </c>
       <c r="J34" s="3"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="6"/>
+      <c r="K34" s="5">
+        <v>161</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="N34" s="5">
+        <v>15</v>
+      </c>
+      <c r="O34" s="6">
+        <v>35.9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="5"/>
+      <c r="A35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="5">
+        <v>50</v>
+      </c>
       <c r="J35" s="3"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="6"/>
+      <c r="K35" s="5">
+        <v>49</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="N35" s="5">
+        <v>14</v>
+      </c>
+      <c r="O35" s="6">
+        <v>2.65</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="5"/>
+      <c r="A36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I36" s="5">
+        <v>50</v>
+      </c>
       <c r="J36" s="3"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="6"/>
+      <c r="K36" s="5">
+        <v>46</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="N36" s="5">
+        <v>18</v>
+      </c>
+      <c r="O36" s="6">
+        <v>3.2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="5"/>
+      <c r="A37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" s="5">
+        <v>50</v>
+      </c>
       <c r="J37" s="3"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="6"/>
+      <c r="K37" s="5">
+        <v>63</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="N37" s="5">
+        <v>18</v>
+      </c>
+      <c r="O37" s="6">
+        <v>32.7</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="5"/>
+      <c r="A38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I38" s="5">
+        <v>50</v>
+      </c>
       <c r="J38" s="3"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="6"/>
+      <c r="K38" s="5">
+        <v>480</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="N38" s="5">
+        <v>16</v>
+      </c>
+      <c r="O38" s="6">
+        <v>68.9</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="3"/>

</xml_diff>

<commit_message>
first run on half the dataset
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="133">
   <si>
     <t>Data Used</t>
   </si>
@@ -404,6 +404,15 @@
   </si>
   <si>
     <t>35.3 &amp; 34.9</t>
+  </si>
+  <si>
+    <t>14006 x 1081</t>
+  </si>
+  <si>
+    <t>84.2 &amp; 72.5</t>
+  </si>
+  <si>
+    <t>79.7 &amp; 71.0</t>
   </si>
 </sst>
 </file>
@@ -411,7 +420,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +438,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -460,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -478,6 +493,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -791,27 +812,27 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O49"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2523,23 +2544,51 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="5"/>
+      <c r="A39" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I39" s="5">
+        <v>50</v>
+      </c>
       <c r="J39" s="3"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
+      <c r="K39" s="5">
+        <v>115</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="N39" s="5">
+        <v>20</v>
+      </c>
+      <c r="O39" s="6">
+        <v>62.8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2548,13 +2597,166 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="5"/>
+      <c r="I40" s="7"/>
       <c r="J40" s="3"/>
-      <c r="K40" s="5"/>
+      <c r="K40" s="7"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="6"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="7"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="7"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ran 50% data and recorded results
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -420,7 +420,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,12 +438,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -495,10 +489,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">

</xml_diff>

<commit_message>
ran with limited alpha, improved distribution but seperation is terrible
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="135">
   <si>
     <t>Data Used</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>79.7 &amp; 71.0</t>
+  </si>
+  <si>
+    <t>87.1 &amp; 82,2</t>
+  </si>
+  <si>
+    <t>76.3 &amp; 72.9</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -438,6 +444,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -489,10 +501,10 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -2583,21 +2595,49 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="7"/>
+      <c r="A40" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I40" s="5">
+        <v>50</v>
+      </c>
       <c r="J40" s="3"/>
-      <c r="K40" s="7"/>
-      <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
-      <c r="N40" s="7"/>
-      <c r="O40" s="8"/>
+      <c r="K40" s="7">
+        <v>374</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="N40" s="7">
+        <v>8</v>
+      </c>
+      <c r="O40" s="8">
+        <v>1.41</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3"/>

</xml_diff>

<commit_message>
edited scripts and added job run results
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="138">
   <si>
     <t>Data Used</t>
   </si>
@@ -419,6 +419,15 @@
   </si>
   <si>
     <t>76.3 &amp; 72.9</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>-211.7 &amp; -59.8</t>
+  </si>
+  <si>
+    <t>47.7 &amp; 45.3</t>
   </si>
 </sst>
 </file>
@@ -426,7 +435,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -444,12 +453,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -481,7 +484,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -499,12 +502,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -824,21 +821,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="17.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="23.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="12.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="8" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2594,7 +2591,7 @@
         <v>62.8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="3" t="s">
         <v>24</v>
       </c>
@@ -2623,7 +2620,7 @@
         <v>50</v>
       </c>
       <c r="J40" s="3"/>
-      <c r="K40" s="7">
+      <c r="K40" s="5">
         <v>374</v>
       </c>
       <c r="L40" s="3" t="s">
@@ -2632,14 +2629,14 @@
       <c r="M40" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="N40" s="7">
+      <c r="N40" s="5">
         <v>8</v>
       </c>
-      <c r="O40" s="8">
+      <c r="O40" s="6">
         <v>1.41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2648,30 +2645,58 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="7"/>
+      <c r="I41" s="5"/>
       <c r="J41" s="3"/>
-      <c r="K41" s="7"/>
+      <c r="K41" s="5"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="8"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="7"/>
+      <c r="A42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I42" s="5">
+        <v>25</v>
+      </c>
       <c r="J42" s="3"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="8"/>
+      <c r="K42" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="N42" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3"/>
@@ -2682,13 +2707,13 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="7"/>
+      <c r="I43" s="5"/>
       <c r="J43" s="3"/>
-      <c r="K43" s="7"/>
+      <c r="K43" s="5"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
-      <c r="N43" s="7"/>
-      <c r="O43" s="8"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3"/>
@@ -2699,13 +2724,13 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="7"/>
+      <c r="I44" s="5"/>
       <c r="J44" s="3"/>
-      <c r="K44" s="7"/>
+      <c r="K44" s="5"/>
       <c r="L44" s="3"/>
       <c r="M44" s="3"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="8"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3"/>
@@ -2716,13 +2741,13 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="7"/>
+      <c r="I45" s="5"/>
       <c r="J45" s="3"/>
-      <c r="K45" s="7"/>
+      <c r="K45" s="5"/>
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
-      <c r="N45" s="7"/>
-      <c r="O45" s="8"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3"/>
@@ -2733,13 +2758,13 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="7"/>
+      <c r="I46" s="5"/>
       <c r="J46" s="3"/>
-      <c r="K46" s="7"/>
+      <c r="K46" s="5"/>
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
-      <c r="N46" s="7"/>
-      <c r="O46" s="8"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="3"/>
@@ -2750,13 +2775,13 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="7"/>
+      <c r="I47" s="5"/>
       <c r="J47" s="3"/>
-      <c r="K47" s="7"/>
+      <c r="K47" s="5"/>
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
-      <c r="N47" s="7"/>
-      <c r="O47" s="8"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="3"/>
@@ -2767,13 +2792,13 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="7"/>
+      <c r="I48" s="5"/>
       <c r="J48" s="3"/>
-      <c r="K48" s="7"/>
+      <c r="K48" s="5"/>
       <c r="L48" s="3"/>
       <c r="M48" s="3"/>
-      <c r="N48" s="7"/>
-      <c r="O48" s="8"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="3"/>

</xml_diff>

<commit_message>
normalizing mapped X between runs didnt really help
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="143">
   <si>
     <t>Data Used</t>
   </si>
@@ -58,6 +58,9 @@
     <t>Alpha</t>
   </si>
   <si>
+    <t>Notes</t>
+  </si>
+  <si>
     <t>bb_data.csv</t>
   </si>
   <si>
@@ -428,6 +431,18 @@
   </si>
   <si>
     <t>47.7 &amp; 45.3</t>
+  </si>
+  <si>
+    <t>iter_cPCA</t>
+  </si>
+  <si>
+    <t>-256.1 &amp; -67.7</t>
+  </si>
+  <si>
+    <t>52.6 &amp; 50.5</t>
+  </si>
+  <si>
+    <t>normalize mappedX in each sub batch</t>
   </si>
 </sst>
 </file>
@@ -815,7 +830,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -835,7 +850,8 @@
     <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
     <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="9" width="6.2907142857142855" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -882,31 +898,34 @@
       <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="P1" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I2" s="5">
         <v>10</v>
@@ -916,40 +935,41 @@
         <v>22</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N2" s="5">
         <v>8</v>
       </c>
       <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="5">
         <v>50</v>
@@ -959,10 +979,10 @@
         <v>88</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N3" s="5">
         <v>18</v>
@@ -970,31 +990,32 @@
       <c r="O3" s="6">
         <v>47.5</v>
       </c>
+      <c r="P3" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I4" s="5">
         <v>25</v>
@@ -1004,10 +1025,10 @@
         <v>91</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N4" s="5">
         <v>17</v>
@@ -1015,31 +1036,32 @@
       <c r="O4" s="6">
         <v>47.5</v>
       </c>
+      <c r="P4" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I5" s="5">
         <v>25</v>
@@ -1049,10 +1071,10 @@
         <v>105</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="N5" s="5">
         <v>17</v>
@@ -1060,31 +1082,32 @@
       <c r="O5" s="6">
         <v>11.8</v>
       </c>
+      <c r="P5" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I6" s="5">
         <v>10</v>
@@ -1094,10 +1117,10 @@
         <v>55</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="N6" s="5">
         <v>9</v>
@@ -1105,31 +1128,32 @@
       <c r="O6" s="6">
         <v>75.6</v>
       </c>
+      <c r="P6" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I7" s="5">
         <v>50</v>
@@ -1139,10 +1163,10 @@
         <v>87</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="N7" s="5">
         <v>18</v>
@@ -1150,31 +1174,32 @@
       <c r="O7" s="6">
         <v>47.5081</v>
       </c>
+      <c r="P7" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I8" s="5">
         <v>50</v>
@@ -1184,10 +1209,10 @@
         <v>63</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N8" s="5">
         <v>18</v>
@@ -1195,31 +1220,32 @@
       <c r="O8" s="6">
         <v>11.77</v>
       </c>
+      <c r="P8" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I9" s="5">
         <v>50</v>
@@ -1229,10 +1255,10 @@
         <v>37</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="N9" s="5">
         <v>17</v>
@@ -1240,31 +1266,32 @@
       <c r="O9" s="6">
         <v>3.51</v>
       </c>
+      <c r="P9" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I10" s="5">
         <v>50</v>
@@ -1274,10 +1301,10 @@
         <v>429</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N10" s="5">
         <v>16</v>
@@ -1285,31 +1312,32 @@
       <c r="O10" s="6">
         <v>57.2</v>
       </c>
+      <c r="P10" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I11" s="5">
         <v>50</v>
@@ -1319,10 +1347,10 @@
         <v>260</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N11" s="5">
         <v>15</v>
@@ -1330,31 +1358,32 @@
       <c r="O11" s="6">
         <v>68.9</v>
       </c>
+      <c r="P11" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I12" s="5">
         <v>50</v>
@@ -1364,10 +1393,10 @@
         <v>440</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N12" s="5">
         <v>17</v>
@@ -1375,31 +1404,32 @@
       <c r="O12" s="6">
         <v>47.5</v>
       </c>
+      <c r="P12" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I13" s="5">
         <v>50</v>
@@ -1409,10 +1439,10 @@
         <v>439</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="N13" s="5">
         <v>17</v>
@@ -1420,31 +1450,32 @@
       <c r="O13" s="6">
         <v>43.3</v>
       </c>
+      <c r="P13" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I14" s="5">
         <v>10</v>
@@ -1454,10 +1485,10 @@
         <v>405</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N14" s="5">
         <v>8</v>
@@ -1465,31 +1496,32 @@
       <c r="O14" s="6">
         <v>9.8</v>
       </c>
+      <c r="P14" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I15" s="5">
         <v>50</v>
@@ -1499,10 +1531,10 @@
         <v>440</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="N15" s="5">
         <v>16</v>
@@ -1510,31 +1542,32 @@
       <c r="O15" s="6">
         <v>24.8</v>
       </c>
+      <c r="P15" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I16" s="5">
         <v>50</v>
@@ -1544,10 +1577,10 @@
         <v>454</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N16" s="5">
         <v>16</v>
@@ -1555,31 +1588,32 @@
       <c r="O16" s="6">
         <v>27.2</v>
       </c>
+      <c r="P16" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I17" s="5">
         <v>50</v>
@@ -1589,10 +1623,10 @@
         <v>437</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N17" s="5">
         <v>16</v>
@@ -1600,31 +1634,32 @@
       <c r="O17" s="6">
         <v>32.7</v>
       </c>
+      <c r="P17" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I18" s="5">
         <v>50</v>
@@ -1634,10 +1669,10 @@
         <v>51</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N18" s="5">
         <v>18</v>
@@ -1645,31 +1680,32 @@
       <c r="O18" s="6">
         <v>4.23</v>
       </c>
+      <c r="P18" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I19" s="5">
         <v>50</v>
@@ -1679,10 +1715,10 @@
         <v>3</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="N19" s="5">
         <v>3</v>
@@ -1690,31 +1726,32 @@
       <c r="O19" s="6">
         <v>1.21</v>
       </c>
+      <c r="P19" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I20" s="5">
         <v>50</v>
@@ -1724,10 +1761,10 @@
         <v>3</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="N20" s="5">
         <v>3</v>
@@ -1735,31 +1772,32 @@
       <c r="O20" s="6">
         <v>1.18</v>
       </c>
+      <c r="P20" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I21" s="5">
         <v>50</v>
@@ -1769,10 +1807,10 @@
         <v>2</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="N21" s="5">
         <v>3</v>
@@ -1780,31 +1818,32 @@
       <c r="O21" s="6">
         <v>0.31</v>
       </c>
+      <c r="P21" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I22" s="5">
         <v>50</v>
@@ -1814,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="N22" s="5">
         <v>3</v>
@@ -1825,31 +1864,32 @@
       <c r="O22" s="6">
         <v>1.02</v>
       </c>
+      <c r="P22" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I23" s="5">
         <v>50</v>
@@ -1859,10 +1899,10 @@
         <v>1</v>
       </c>
       <c r="L23" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="N23" s="5">
         <v>2</v>
@@ -1870,31 +1910,32 @@
       <c r="O23" s="6">
         <v>1.5</v>
       </c>
+      <c r="P23" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I24" s="5">
         <v>50</v>
@@ -1904,10 +1945,10 @@
         <v>1</v>
       </c>
       <c r="L24" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="N24" s="5">
         <v>2</v>
@@ -1915,31 +1956,32 @@
       <c r="O24" s="6">
         <v>1.45</v>
       </c>
+      <c r="P24" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I25" s="5">
         <v>50</v>
@@ -1949,10 +1991,10 @@
         <v>1</v>
       </c>
       <c r="L25" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="N25" s="5">
         <v>2</v>
@@ -1960,31 +2002,32 @@
       <c r="O25" s="6">
         <v>1.3</v>
       </c>
+      <c r="P25" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I26" s="5">
         <v>50</v>
@@ -1994,10 +2037,10 @@
         <v>1</v>
       </c>
       <c r="L26" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="N26" s="5">
         <v>2</v>
@@ -2005,31 +2048,32 @@
       <c r="O26" s="6">
         <v>0.01</v>
       </c>
+      <c r="P26" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I27" s="5">
         <v>50</v>
@@ -2039,10 +2083,10 @@
         <v>102</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N27" s="5">
         <v>19</v>
@@ -2050,31 +2094,32 @@
       <c r="O27" s="6">
         <v>52.1</v>
       </c>
+      <c r="P27" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I28" s="5">
         <v>50</v>
@@ -2084,10 +2129,10 @@
         <v>85</v>
       </c>
       <c r="L28" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N28" s="5">
         <v>18</v>
@@ -2095,31 +2140,32 @@
       <c r="O28" s="6">
         <v>15.6</v>
       </c>
+      <c r="P28" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I29" s="5">
         <v>50</v>
@@ -2129,10 +2175,10 @@
         <v>51</v>
       </c>
       <c r="L29" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N29" s="5">
         <v>17</v>
@@ -2140,31 +2186,32 @@
       <c r="O29" s="6">
         <v>2.66</v>
       </c>
+      <c r="P29" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I30" s="5">
         <v>50</v>
@@ -2174,10 +2221,10 @@
         <v>114</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="N30" s="5">
         <v>19</v>
@@ -2185,31 +2232,32 @@
       <c r="O30" s="6">
         <v>68.9</v>
       </c>
+      <c r="P30" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I31" s="5">
         <v>50</v>
@@ -2219,10 +2267,10 @@
         <v>54</v>
       </c>
       <c r="L31" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N31" s="5">
         <v>18</v>
@@ -2230,31 +2278,32 @@
       <c r="O31" s="6">
         <v>12.9</v>
       </c>
+      <c r="P31" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I32" s="5">
         <v>50</v>
@@ -2264,10 +2313,10 @@
         <v>243</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N32" s="5">
         <v>16</v>
@@ -2275,31 +2324,32 @@
       <c r="O32" s="6">
         <v>68.9</v>
       </c>
+      <c r="P32" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I33" s="5">
         <v>50</v>
@@ -2309,10 +2359,10 @@
         <v>386</v>
       </c>
       <c r="L33" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="N33" s="5">
         <v>17</v>
@@ -2320,31 +2370,32 @@
       <c r="O33" s="6">
         <v>75.6</v>
       </c>
+      <c r="P33" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I34" s="5">
         <v>50</v>
@@ -2354,10 +2405,10 @@
         <v>161</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="N34" s="5">
         <v>15</v>
@@ -2365,31 +2416,32 @@
       <c r="O34" s="6">
         <v>35.9</v>
       </c>
+      <c r="P34" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
       <c r="A35" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I35" s="5">
         <v>50</v>
@@ -2399,10 +2451,10 @@
         <v>49</v>
       </c>
       <c r="L35" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N35" s="5">
         <v>14</v>
@@ -2410,31 +2462,32 @@
       <c r="O35" s="6">
         <v>2.65</v>
       </c>
+      <c r="P35" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
       <c r="A36" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I36" s="5">
         <v>50</v>
@@ -2444,10 +2497,10 @@
         <v>46</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="N36" s="5">
         <v>18</v>
@@ -2455,31 +2508,32 @@
       <c r="O36" s="6">
         <v>3.2</v>
       </c>
+      <c r="P36" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I37" s="5">
         <v>50</v>
@@ -2489,10 +2543,10 @@
         <v>63</v>
       </c>
       <c r="L37" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="N37" s="5">
         <v>18</v>
@@ -2500,31 +2554,32 @@
       <c r="O37" s="6">
         <v>32.7</v>
       </c>
+      <c r="P37" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I38" s="5">
         <v>50</v>
@@ -2534,10 +2589,10 @@
         <v>480</v>
       </c>
       <c r="L38" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="N38" s="5">
         <v>16</v>
@@ -2545,31 +2600,32 @@
       <c r="O38" s="6">
         <v>68.9</v>
       </c>
+      <c r="P38" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I39" s="5">
         <v>50</v>
@@ -2579,10 +2635,10 @@
         <v>115</v>
       </c>
       <c r="L39" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="N39" s="5">
         <v>20</v>
@@ -2590,31 +2646,32 @@
       <c r="O39" s="6">
         <v>62.8</v>
       </c>
+      <c r="P39" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I40" s="5">
         <v>50</v>
@@ -2624,10 +2681,10 @@
         <v>374</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="N40" s="5">
         <v>8</v>
@@ -2635,6 +2692,7 @@
       <c r="O40" s="6">
         <v>1.41</v>
       </c>
+      <c r="P40" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="3"/>
@@ -2652,68 +2710,103 @@
       <c r="M41" s="3"/>
       <c r="N41" s="5"/>
       <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I42" s="5">
         <v>25</v>
       </c>
       <c r="J42" s="3"/>
       <c r="K42" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="L42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="N42" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="M42" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="N42" s="5" t="s">
-        <v>135</v>
-      </c>
       <c r="O42" s="5" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="P42" s="5" t="s">
+        <v>139</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="5"/>
+      <c r="A43" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I43" s="5">
+        <v>25</v>
+      </c>
       <c r="J43" s="3"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="6"/>
+      <c r="K43" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="N43" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3"/>
@@ -2731,6 +2824,7 @@
       <c r="M44" s="3"/>
       <c r="N44" s="5"/>
       <c r="O44" s="6"/>
+      <c r="P44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3"/>
@@ -2748,6 +2842,7 @@
       <c r="M45" s="3"/>
       <c r="N45" s="5"/>
       <c r="O45" s="6"/>
+      <c r="P45" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3"/>
@@ -2765,6 +2860,7 @@
       <c r="M46" s="3"/>
       <c r="N46" s="5"/>
       <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="3"/>
@@ -2782,6 +2878,7 @@
       <c r="M47" s="3"/>
       <c r="N47" s="5"/>
       <c r="O47" s="6"/>
+      <c r="P47" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="3"/>
@@ -2799,6 +2896,7 @@
       <c r="M48" s="3"/>
       <c r="N48" s="5"/>
       <c r="O48" s="6"/>
+      <c r="P48" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="3"/>
@@ -2816,6 +2914,7 @@
       <c r="M49" s="3"/>
       <c r="N49" s="5"/>
       <c r="O49" s="6"/>
+      <c r="P49" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
incorporated R post processing into shell script full pipeline, also updated some job run results
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="146">
   <si>
     <t>Data Used</t>
   </si>
@@ -443,6 +443,15 @@
   </si>
   <si>
     <t>normalize mappedX in each sub batch</t>
+  </si>
+  <si>
+    <t>25.4 &amp; 18.8</t>
+  </si>
+  <si>
+    <t>33.9 &amp; 29.4</t>
+  </si>
+  <si>
+    <t>filter out large V_sort</t>
   </si>
 </sst>
 </file>
@@ -2809,22 +2818,52 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="5"/>
+      <c r="A44" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="5">
+        <v>25</v>
+      </c>
       <c r="J44" s="3"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
+      <c r="K44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="N44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="P44" s="6" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3"/>

</xml_diff>

<commit_message>
cPC entire normalization actually improves results a bit, so keep it in the pipeline, also modified post processing script to not generate graphs
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="149">
   <si>
     <t>Data Used</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>filter out large V_sort</t>
+  </si>
+  <si>
+    <t>-198.2% &amp; -63.2%</t>
+  </si>
+  <si>
+    <t>47.6 &amp; 44.5</t>
+  </si>
+  <si>
+    <t>normalize cPC in each sub batch</t>
   </si>
 </sst>
 </file>
@@ -508,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -528,6 +537,9 @@
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
@@ -535,6 +547,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -845,22 +860,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="8" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="8" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="9" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="8" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="11" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -907,7 +922,7 @@
       <c r="O1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2721,7 +2736,7 @@
       <c r="O41" s="6"/>
       <c r="P41" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
       <c r="A42" s="3" t="s">
         <v>25</v>
       </c>
@@ -2762,14 +2777,14 @@
       <c r="N42" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="O42" s="5" t="s">
+      <c r="O42" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P42" s="5" t="s">
+      <c r="P42" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="3" t="s">
         <v>25</v>
       </c>
@@ -2810,14 +2825,14 @@
       <c r="N43" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="O43" s="5" t="s">
+      <c r="O43" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P43" s="6" t="s">
+      <c r="P43" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="3" t="s">
         <v>25</v>
       </c>
@@ -2858,30 +2873,60 @@
       <c r="N44" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="O44" s="5" t="s">
+      <c r="O44" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P44" s="6" t="s">
+      <c r="P44" s="7" t="s">
         <v>145</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="5"/>
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
+      <c r="A45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="5">
+        <v>25</v>
+      </c>
       <c r="J45" s="3"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
+      <c r="K45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N45" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P45" s="6" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3"/>

</xml_diff>

<commit_message>
ran with 20 batches, results are actually pretty good
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="152">
   <si>
     <t>Data Used</t>
   </si>
@@ -454,13 +454,22 @@
     <t>filter out large V_sort</t>
   </si>
   <si>
-    <t>-198.2% &amp; -63.2%</t>
+    <t>-198.2 &amp; -63.2</t>
   </si>
   <si>
     <t>47.6 &amp; 44.5</t>
   </si>
   <si>
     <t>normalize cPC in each sub batch</t>
+  </si>
+  <si>
+    <t>-55.6 &amp; -27.9</t>
+  </si>
+  <si>
+    <t>13.7 &amp; 11.3</t>
+  </si>
+  <si>
+    <t>20 batches</t>
   </si>
 </sst>
 </file>
@@ -2924,29 +2933,59 @@
       <c r="O45" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P45" s="6" t="s">
+      <c r="P45" s="7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="5"/>
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
+      <c r="A46" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="5">
+        <v>25</v>
+      </c>
       <c r="J46" s="3"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="6"/>
-      <c r="P46" s="6"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+      <c r="K46" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="N46" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O46" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P46" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -2964,7 +3003,7 @@
       <c r="O47" s="6"/>
       <c r="P47" s="6"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>

</xml_diff>

<commit_message>
ran with 15 batches, also modified post processing script to not produce plots
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="155">
   <si>
     <t>Data Used</t>
   </si>
@@ -470,6 +470,15 @@
   </si>
   <si>
     <t>20 batches</t>
+  </si>
+  <si>
+    <t>-55.4 &amp; -27.7</t>
+  </si>
+  <si>
+    <t>13.8 &amp; 11.4</t>
+  </si>
+  <si>
+    <t>15 batches</t>
   </si>
 </sst>
 </file>
@@ -526,7 +535,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -547,6 +556,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -863,28 +881,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="12" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="13" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -2981,27 +2999,57 @@
       <c r="O46" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P46" s="6" t="s">
+      <c r="P46" s="7" t="s">
         <v>151</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="5"/>
+      <c r="A47" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="5">
+        <v>25</v>
+      </c>
       <c r="J47" s="3"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
+      <c r="K47" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="N47" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P47" s="6" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="3"/>
@@ -3030,14 +3078,158 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="5"/>
+      <c r="I49" s="8"/>
       <c r="J49" s="3"/>
-      <c r="K49" s="5"/>
+      <c r="K49" s="8"/>
       <c r="L49" s="3"/>
       <c r="M49" s="3"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
+      <c r="N49" s="8"/>
+      <c r="O49" s="9"/>
+      <c r="P49" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="8"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="8"/>
+      <c r="O50" s="9"/>
+      <c r="P50" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="8"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="8"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="8"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="8"/>
+      <c r="O52" s="9"/>
+      <c r="P52" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="8"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="8"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="8"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="8"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="8"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="8"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="9"/>
+      <c r="P56" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added a couple more tests for sub batching
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="169">
   <si>
     <t>Data Used</t>
   </si>
@@ -433,7 +433,7 @@
     <t>47.7 &amp; 45.3</t>
   </si>
   <si>
-    <t>iter_cPCA</t>
+    <t>iter_cPCA 10 batches</t>
   </si>
   <si>
     <t>-256.1 &amp; -67.7</t>
@@ -488,6 +488,39 @@
   </si>
   <si>
     <t>5 batches</t>
+  </si>
+  <si>
+    <t>-18.5 &amp; -5</t>
+  </si>
+  <si>
+    <t>-27.6 &amp; -18.4</t>
+  </si>
+  <si>
+    <t>10 batches</t>
+  </si>
+  <si>
+    <t>21.0 &amp; 7.2</t>
+  </si>
+  <si>
+    <t>-118.8 &amp; -51.8</t>
+  </si>
+  <si>
+    <t>-136 &amp; -49.3</t>
+  </si>
+  <si>
+    <t>19.6 &amp; 16.9</t>
+  </si>
+  <si>
+    <t>15 batches (shuffled data)</t>
+  </si>
+  <si>
+    <t>-45.6 &amp; -22.2</t>
+  </si>
+  <si>
+    <t>4.9 &amp; 4.2</t>
+  </si>
+  <si>
+    <t>25 batches</t>
   </si>
 </sst>
 </file>
@@ -495,7 +528,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -513,12 +546,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -550,7 +577,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -571,15 +598,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -902,22 +920,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="14" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="8" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="8" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="8" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="8" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="10" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="11" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3114,77 +3132,197 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="8"/>
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
+      <c r="A49" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="5">
+        <v>25</v>
+      </c>
       <c r="J49" s="3"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="9"/>
-      <c r="P49" s="10"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="8"/>
+      <c r="K49" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="N49" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O49" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P49" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
+      <c r="A50" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="5">
+        <v>25</v>
+      </c>
       <c r="J50" s="3"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="8"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="10"/>
+      <c r="K50" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O50" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P50" s="7" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="8"/>
+      <c r="A51" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="5">
+        <v>25</v>
+      </c>
       <c r="J51" s="3"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="8"/>
-      <c r="O51" s="9"/>
-      <c r="P51" s="10"/>
+      <c r="K51" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="8"/>
+      <c r="A52" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="5">
+        <v>25</v>
+      </c>
       <c r="J52" s="3"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="8"/>
-      <c r="O52" s="9"/>
-      <c r="P52" s="10"/>
+      <c r="K52" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P52" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="3"/>
@@ -3195,14 +3333,14 @@
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
-      <c r="I53" s="8"/>
+      <c r="I53" s="5"/>
       <c r="J53" s="3"/>
-      <c r="K53" s="8"/>
+      <c r="K53" s="5"/>
       <c r="L53" s="3"/>
       <c r="M53" s="3"/>
-      <c r="N53" s="8"/>
-      <c r="O53" s="9"/>
-      <c r="P53" s="10"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="3"/>
@@ -3213,14 +3351,14 @@
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
-      <c r="I54" s="8"/>
+      <c r="I54" s="5"/>
       <c r="J54" s="3"/>
-      <c r="K54" s="8"/>
+      <c r="K54" s="5"/>
       <c r="L54" s="3"/>
       <c r="M54" s="3"/>
-      <c r="N54" s="8"/>
-      <c r="O54" s="9"/>
-      <c r="P54" s="10"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="6"/>
+      <c r="P54" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="3"/>
@@ -3231,14 +3369,14 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="8"/>
+      <c r="I55" s="5"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="8"/>
+      <c r="K55" s="5"/>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
-      <c r="N55" s="8"/>
-      <c r="O55" s="9"/>
-      <c r="P55" s="10"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="3"/>
@@ -3249,14 +3387,14 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="8"/>
+      <c r="I56" s="5"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="8"/>
+      <c r="K56" s="5"/>
       <c r="L56" s="3"/>
       <c r="M56" s="3"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="10"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="3"/>

</xml_diff>

<commit_message>
tuned lambda threshold, this didnt make that much of a difference
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="181">
   <si>
     <t>Data Used</t>
   </si>
@@ -539,6 +539,24 @@
   </si>
   <si>
     <t>as above but filter out large V_sort</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 47.5</t>
+  </si>
+  <si>
+    <t>change lambda &gt; 0.001</t>
+  </si>
+  <si>
+    <t>102.8 &amp; 101.6</t>
+  </si>
+  <si>
+    <t>80 &amp; 80.9</t>
+  </si>
+  <si>
+    <t>change lambda &gt; 0.01</t>
   </si>
 </sst>
 </file>
@@ -947,7 +965,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P59"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -3389,7 +3407,7 @@
         <v>18</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>20</v>
@@ -3435,7 +3453,7 @@
         <v>18</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>20</v>
@@ -3468,40 +3486,96 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="8"/>
+      <c r="A56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="5">
+        <v>250</v>
+      </c>
       <c r="J56" s="3"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="8"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="10"/>
+      <c r="K56" s="5"/>
+      <c r="L56" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="N56" s="5">
+        <v>227</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="P56" s="7" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="8"/>
+      <c r="A57" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I57" s="5">
+        <v>250</v>
+      </c>
       <c r="J57" s="3"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="8"/>
-      <c r="O57" s="9"/>
-      <c r="P57" s="10"/>
+      <c r="K57" s="5"/>
+      <c r="L57" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="N57" s="5">
+        <v>17</v>
+      </c>
+      <c r="O57" s="6">
+        <v>5.09</v>
+      </c>
+      <c r="P57" s="7" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="3"/>
@@ -3512,14 +3586,14 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="5"/>
+      <c r="I58" s="8"/>
       <c r="J58" s="3"/>
-      <c r="K58" s="5"/>
+      <c r="K58" s="8"/>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="6"/>
-      <c r="P58" s="7"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="9"/>
+      <c r="P58" s="10"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="3"/>
@@ -3530,14 +3604,104 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="5"/>
+      <c r="I59" s="8"/>
       <c r="J59" s="3"/>
-      <c r="K59" s="5"/>
+      <c r="K59" s="8"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="6"/>
-      <c r="P59" s="6"/>
+      <c r="N59" s="8"/>
+      <c r="O59" s="9"/>
+      <c r="P59" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="8"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="8"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="8"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="8"/>
+      <c r="O61" s="9"/>
+      <c r="P61" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="8"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="8"/>
+      <c r="O62" s="9"/>
+      <c r="P62" s="10"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="5"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="6"/>
+      <c r="P63" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="5"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="6"/>
+      <c r="P64" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
revert back to old versions for cPCA iteratively running
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="188">
   <si>
     <t>Data Used</t>
   </si>
@@ -569,6 +569,15 @@
   </si>
   <si>
     <t>only chamge lambda &gt; 0.01, nothing else</t>
+  </si>
+  <si>
+    <t>5602 x 1081</t>
+  </si>
+  <si>
+    <t>feature selection 0.95</t>
+  </si>
+  <si>
+    <t>feature selection 0.5</t>
   </si>
 </sst>
 </file>
@@ -3621,40 +3630,96 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="5"/>
+      <c r="A59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="5">
+        <v>25</v>
+      </c>
       <c r="J59" s="3"/>
       <c r="K59" s="5"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="6"/>
-      <c r="P59" s="7"/>
+      <c r="L59" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="N59" s="5">
+        <v>20</v>
+      </c>
+      <c r="O59" s="6">
+        <v>3.85</v>
+      </c>
+      <c r="P59" s="7" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="5"/>
+      <c r="A60" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I60" s="5">
+        <v>25</v>
+      </c>
       <c r="J60" s="3"/>
       <c r="K60" s="5"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="6"/>
-      <c r="P60" s="7"/>
+      <c r="L60" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="N60" s="5">
+        <v>11</v>
+      </c>
+      <c r="O60" s="6">
+        <v>91.1</v>
+      </c>
+      <c r="P60" s="7" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="3"/>

</xml_diff>

<commit_message>
fixed path in trajectory python code
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="190">
   <si>
     <t>Data Used</t>
   </si>
@@ -521,6 +521,12 @@
   </si>
   <si>
     <t>25 batches</t>
+  </si>
+  <si>
+    <t>-27.4 &amp; -10.3</t>
+  </si>
+  <si>
+    <t>22.2 &amp; 13.0</t>
   </si>
   <si>
     <t>74.5 &amp; 52.4</t>
@@ -634,7 +640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -655,6 +661,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -971,28 +986,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="9" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="8" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="9" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="8" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="8" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="9" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="10" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="11" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="11" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="11" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="11" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="11" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="11" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="12" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="13" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="14" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3381,25 +3396,55 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="5"/>
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+      <c r="A53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I53" s="5">
+        <v>25</v>
+      </c>
       <c r="J53" s="3"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="6"/>
-      <c r="P53" s="7"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+      <c r="K53" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="N53" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P53" s="8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3" t="s">
         <v>25</v>
       </c>
@@ -3428,160 +3473,72 @@
         <v>25</v>
       </c>
       <c r="J54" s="3"/>
-      <c r="K54" s="5"/>
-      <c r="L54" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="M54" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="N54" s="5">
-        <v>2</v>
-      </c>
-      <c r="O54" s="6">
-        <v>5.09</v>
-      </c>
-      <c r="P54" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
-      <c r="A55" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I55" s="5">
-        <v>25</v>
-      </c>
+      <c r="K54" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P54" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="9"/>
       <c r="J55" s="3"/>
-      <c r="K55" s="5"/>
-      <c r="L55" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="M55" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="N55" s="5">
-        <v>2</v>
-      </c>
-      <c r="O55" s="6">
-        <v>4.64</v>
-      </c>
-      <c r="P55" s="7" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
-      <c r="A56" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I56" s="5">
-        <v>250</v>
-      </c>
+      <c r="K55" s="9"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="8"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="9"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="M56" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="N56" s="5">
-        <v>227</v>
-      </c>
-      <c r="O56" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="P56" s="7" t="s">
-        <v>177</v>
-      </c>
+      <c r="K56" s="9"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="9"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
-      <c r="A57" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I57" s="5">
-        <v>250</v>
-      </c>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="5"/>
       <c r="J57" s="3"/>
       <c r="K57" s="5"/>
-      <c r="L57" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="M57" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="N57" s="5">
-        <v>17</v>
-      </c>
-      <c r="O57" s="6">
-        <v>5.09</v>
-      </c>
-      <c r="P57" s="7" t="s">
-        <v>180</v>
-      </c>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="3" t="s">
@@ -3609,24 +3566,24 @@
         <v>22</v>
       </c>
       <c r="I58" s="5">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="J58" s="3"/>
       <c r="K58" s="5"/>
       <c r="L58" s="3" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="N58" s="5">
-        <v>51</v>
-      </c>
-      <c r="O58" s="6" t="s">
-        <v>183</v>
+        <v>2</v>
+      </c>
+      <c r="O58" s="6">
+        <v>5.09</v>
       </c>
       <c r="P58" s="7" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -3634,7 +3591,7 @@
         <v>25</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>17</v>
@@ -3660,19 +3617,19 @@
       <c r="J59" s="3"/>
       <c r="K59" s="5"/>
       <c r="L59" s="3" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="N59" s="5">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="O59" s="6">
-        <v>3.85</v>
+        <v>4.64</v>
       </c>
       <c r="P59" s="7" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
@@ -3680,7 +3637,7 @@
         <v>25</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>185</v>
+        <v>26</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>17</v>
@@ -3701,97 +3658,281 @@
         <v>22</v>
       </c>
       <c r="I60" s="5">
-        <v>25</v>
+        <v>250</v>
       </c>
       <c r="J60" s="3"/>
       <c r="K60" s="5"/>
       <c r="L60" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="N60" s="5">
-        <v>11</v>
-      </c>
-      <c r="O60" s="6">
-        <v>91.1</v>
+        <v>227</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="P60" s="7" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="5"/>
+      <c r="A61" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I61" s="5">
+        <v>250</v>
+      </c>
       <c r="J61" s="3"/>
       <c r="K61" s="5"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="6"/>
-      <c r="P61" s="7"/>
+      <c r="L61" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="N61" s="5">
+        <v>17</v>
+      </c>
+      <c r="O61" s="6">
+        <v>5.09</v>
+      </c>
+      <c r="P61" s="7" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="5"/>
+      <c r="A62" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I62" s="5">
+        <v>100</v>
+      </c>
       <c r="J62" s="3"/>
       <c r="K62" s="5"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="6"/>
-      <c r="P62" s="7"/>
+      <c r="L62" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N62" s="5">
+        <v>51</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="P62" s="7" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="5"/>
+      <c r="A63" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I63" s="5">
+        <v>25</v>
+      </c>
       <c r="J63" s="3"/>
       <c r="K63" s="5"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="6"/>
-      <c r="P63" s="7"/>
+      <c r="L63" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="N63" s="5">
+        <v>20</v>
+      </c>
+      <c r="O63" s="6">
+        <v>3.85</v>
+      </c>
+      <c r="P63" s="7" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="5"/>
+      <c r="A64" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" s="5">
+        <v>25</v>
+      </c>
       <c r="J64" s="3"/>
       <c r="K64" s="5"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="6"/>
-      <c r="P64" s="6"/>
+      <c r="L64" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="M64" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="N64" s="5">
+        <v>11</v>
+      </c>
+      <c r="O64" s="6">
+        <v>91.1</v>
+      </c>
+      <c r="P64" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="6"/>
+      <c r="P65" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="5"/>
+      <c r="O66" s="6"/>
+      <c r="P66" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="5"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="5"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="5"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="5"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="5"/>
+      <c r="O68" s="6"/>
+      <c r="P68" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more results to run
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="193">
   <si>
     <t>Data Used</t>
   </si>
@@ -527,6 +527,15 @@
   </si>
   <si>
     <t>22.2 &amp; 13.0</t>
+  </si>
+  <si>
+    <t>-87.3 &amp; -17.2</t>
+  </si>
+  <si>
+    <t>-11.0 &amp; -6.9</t>
+  </si>
+  <si>
+    <t>12 batches</t>
   </si>
   <si>
     <t>74.5 &amp; 52.4</t>
@@ -591,7 +600,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -609,6 +618,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -663,13 +678,13 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -3396,7 +3411,7 @@
         <v>168</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="3" t="s">
         <v>25</v>
       </c>
@@ -3444,7 +3459,7 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="3" t="s">
         <v>25</v>
       </c>
@@ -3476,33 +3491,65 @@
       <c r="K54" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
+      <c r="L54" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="N54" s="5" t="s">
         <v>136</v>
       </c>
       <c r="O54" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P54" s="8"/>
+      <c r="P54" s="8" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="9"/>
+      <c r="A55" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I55" s="5">
+        <v>25</v>
+      </c>
       <c r="J55" s="3"/>
-      <c r="K55" s="9"/>
+      <c r="K55" s="5" t="s">
+        <v>136</v>
+      </c>
       <c r="L55" s="3"/>
       <c r="M55" s="3"/>
-      <c r="N55" s="9"/>
-      <c r="O55" s="10"/>
-      <c r="P55" s="8"/>
+      <c r="N55" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P55" s="8" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3"/>
@@ -3571,10 +3618,10 @@
       <c r="J58" s="3"/>
       <c r="K58" s="5"/>
       <c r="L58" s="3" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="N58" s="5">
         <v>2</v>
@@ -3583,7 +3630,7 @@
         <v>5.09</v>
       </c>
       <c r="P58" s="7" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -3617,10 +3664,10 @@
       <c r="J59" s="3"/>
       <c r="K59" s="5"/>
       <c r="L59" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N59" s="5">
         <v>2</v>
@@ -3629,7 +3676,7 @@
         <v>4.64</v>
       </c>
       <c r="P59" s="7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
@@ -3663,19 +3710,19 @@
       <c r="J60" s="3"/>
       <c r="K60" s="5"/>
       <c r="L60" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N60" s="5">
         <v>227</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="P60" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
@@ -3709,10 +3756,10 @@
       <c r="J61" s="3"/>
       <c r="K61" s="5"/>
       <c r="L61" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="N61" s="5">
         <v>17</v>
@@ -3721,7 +3768,7 @@
         <v>5.09</v>
       </c>
       <c r="P61" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
@@ -3755,19 +3802,19 @@
       <c r="J62" s="3"/>
       <c r="K62" s="5"/>
       <c r="L62" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N62" s="5">
         <v>51</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="P62" s="7" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
@@ -3775,7 +3822,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>17</v>
@@ -3801,10 +3848,10 @@
       <c r="J63" s="3"/>
       <c r="K63" s="5"/>
       <c r="L63" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N63" s="5">
         <v>20</v>
@@ -3813,7 +3860,7 @@
         <v>3.85</v>
       </c>
       <c r="P63" s="7" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -3821,7 +3868,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>17</v>
@@ -3847,10 +3894,10 @@
       <c r="J64" s="3"/>
       <c r="K64" s="5"/>
       <c r="L64" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="N64" s="5">
         <v>11</v>
@@ -3859,7 +3906,7 @@
         <v>91.1</v>
       </c>
       <c r="P64" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
ran batch of 20 with 160/100 and the results are actually pretty good
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="196">
   <si>
     <t>Data Used</t>
   </si>
@@ -536,6 +536,15 @@
   </si>
   <si>
     <t>12 batches</t>
+  </si>
+  <si>
+    <t>53.1 &amp; 35.5</t>
+  </si>
+  <si>
+    <t>-188 &amp; -65.2</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>74.5 &amp; 52.4</t>
@@ -600,7 +609,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,12 +627,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -655,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -678,14 +681,8 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -1007,22 +1004,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="11" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="11" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="11" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="11" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="11" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="12" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="11" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="12" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="11" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="11" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="12" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="13" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="14" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="11" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="12" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3455,7 +3452,7 @@
       <c r="O53" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P53" s="8" t="s">
+      <c r="P53" s="7" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3503,11 +3500,11 @@
       <c r="O54" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P54" s="8" t="s">
+      <c r="P54" s="7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="3" t="s">
         <v>25</v>
       </c>
@@ -3539,19 +3536,23 @@
       <c r="K55" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
+      <c r="L55" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>175</v>
+      </c>
       <c r="N55" s="5" t="s">
         <v>136</v>
       </c>
       <c r="O55" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P55" s="8" t="s">
+      <c r="P55" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -3560,14 +3561,16 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="9"/>
+      <c r="I56" s="5"/>
       <c r="J56" s="3"/>
-      <c r="K56" s="9"/>
+      <c r="K56" s="5"/>
       <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="9"/>
-      <c r="O56" s="10"/>
-      <c r="P56" s="8"/>
+      <c r="M56" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="N56" s="5"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="3"/>
@@ -3618,10 +3621,10 @@
       <c r="J58" s="3"/>
       <c r="K58" s="5"/>
       <c r="L58" s="3" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="N58" s="5">
         <v>2</v>
@@ -3630,7 +3633,7 @@
         <v>5.09</v>
       </c>
       <c r="P58" s="7" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -3664,10 +3667,10 @@
       <c r="J59" s="3"/>
       <c r="K59" s="5"/>
       <c r="L59" s="3" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="N59" s="5">
         <v>2</v>
@@ -3676,7 +3679,7 @@
         <v>4.64</v>
       </c>
       <c r="P59" s="7" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
@@ -3710,19 +3713,19 @@
       <c r="J60" s="3"/>
       <c r="K60" s="5"/>
       <c r="L60" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="N60" s="5">
         <v>227</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="P60" s="7" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
@@ -3756,10 +3759,10 @@
       <c r="J61" s="3"/>
       <c r="K61" s="5"/>
       <c r="L61" s="3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="N61" s="5">
         <v>17</v>
@@ -3768,7 +3771,7 @@
         <v>5.09</v>
       </c>
       <c r="P61" s="7" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
@@ -3802,19 +3805,19 @@
       <c r="J62" s="3"/>
       <c r="K62" s="5"/>
       <c r="L62" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="N62" s="5">
         <v>51</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="P62" s="7" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
@@ -3822,7 +3825,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>17</v>
@@ -3848,10 +3851,10 @@
       <c r="J63" s="3"/>
       <c r="K63" s="5"/>
       <c r="L63" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="N63" s="5">
         <v>20</v>
@@ -3860,7 +3863,7 @@
         <v>3.85</v>
       </c>
       <c r="P63" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -3868,7 +3871,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>17</v>
@@ -3894,10 +3897,10 @@
       <c r="J64" s="3"/>
       <c r="K64" s="5"/>
       <c r="L64" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="N64" s="5">
         <v>11</v>
@@ -3906,7 +3909,7 @@
         <v>91.1</v>
       </c>
       <c r="P64" s="7" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
added job run results
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="198">
   <si>
     <t>Data Used</t>
   </si>
@@ -542,6 +542,12 @@
   </si>
   <si>
     <t>-188 &amp; -65.2</t>
+  </si>
+  <si>
+    <t>53.8 &amp; 43.4</t>
+  </si>
+  <si>
+    <t>-237.2 &amp; -71.6</t>
   </si>
   <si>
     <t/>
@@ -3553,24 +3559,52 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="5"/>
+      <c r="A56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I56" s="5">
+        <v>25</v>
+      </c>
       <c r="J56" s="3"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="8" t="s">
+      <c r="K56" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L56" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="N56" s="5"/>
-      <c r="O56" s="6"/>
-      <c r="P56" s="7"/>
+      <c r="M56" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="N56" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P56" s="7" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="3"/>
@@ -3584,8 +3618,12 @@
       <c r="I57" s="5"/>
       <c r="J57" s="3"/>
       <c r="K57" s="5"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
+      <c r="L57" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="M57" s="8" t="s">
+        <v>178</v>
+      </c>
       <c r="N57" s="5"/>
       <c r="O57" s="6"/>
       <c r="P57" s="7"/>
@@ -3621,10 +3659,10 @@
       <c r="J58" s="3"/>
       <c r="K58" s="5"/>
       <c r="L58" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="N58" s="5">
         <v>2</v>
@@ -3633,7 +3671,7 @@
         <v>5.09</v>
       </c>
       <c r="P58" s="7" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
@@ -3667,10 +3705,10 @@
       <c r="J59" s="3"/>
       <c r="K59" s="5"/>
       <c r="L59" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="N59" s="5">
         <v>2</v>
@@ -3679,7 +3717,7 @@
         <v>4.64</v>
       </c>
       <c r="P59" s="7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
@@ -3713,19 +3751,19 @@
       <c r="J60" s="3"/>
       <c r="K60" s="5"/>
       <c r="L60" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="N60" s="5">
         <v>227</v>
       </c>
       <c r="O60" s="6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="P60" s="7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
@@ -3759,10 +3797,10 @@
       <c r="J61" s="3"/>
       <c r="K61" s="5"/>
       <c r="L61" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="N61" s="5">
         <v>17</v>
@@ -3771,7 +3809,7 @@
         <v>5.09</v>
       </c>
       <c r="P61" s="7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
@@ -3805,19 +3843,19 @@
       <c r="J62" s="3"/>
       <c r="K62" s="5"/>
       <c r="L62" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N62" s="5">
         <v>51</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="P62" s="7" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
@@ -3825,7 +3863,7 @@
         <v>25</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>17</v>
@@ -3851,10 +3889,10 @@
       <c r="J63" s="3"/>
       <c r="K63" s="5"/>
       <c r="L63" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="N63" s="5">
         <v>20</v>
@@ -3863,7 +3901,7 @@
         <v>3.85</v>
       </c>
       <c r="P63" s="7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -3871,7 +3909,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>17</v>
@@ -3897,10 +3935,10 @@
       <c r="J64" s="3"/>
       <c r="K64" s="5"/>
       <c r="L64" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="N64" s="5">
         <v>11</v>
@@ -3909,7 +3947,7 @@
         <v>91.1</v>
       </c>
       <c r="P64" s="7" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
added more job runs
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="203">
   <si>
     <t>Data Used</t>
   </si>
@@ -530,6 +530,15 @@
   </si>
   <si>
     <t>12 batches</t>
+  </si>
+  <si>
+    <t>15.3 &amp; 7.7</t>
+  </si>
+  <si>
+    <t>70.4 &amp; -34.3</t>
+  </si>
+  <si>
+    <t>13 batches</t>
   </si>
   <si>
     <t>21.0 &amp; 7.2</t>
@@ -621,7 +630,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -639,6 +648,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -670,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -694,6 +709,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1010,28 +1028,28 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="11.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="10.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="10" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="9" width="2.1478571428571427" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="10" width="10.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="9" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="9" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="10" width="7.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="11" width="8.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="12" width="32.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="10" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="11.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="11" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="2.1478571428571427" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="10" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="10" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="11" width="7.576428571428571" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="12" width="8.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="13" width="32.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3468,7 +3486,7 @@
         <v>171</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3" t="s">
         <v>25</v>
       </c>
@@ -3512,11 +3530,11 @@
       <c r="O54" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P54" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+      <c r="P54" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="3" t="s">
         <v>25</v>
       </c>
@@ -3549,10 +3567,10 @@
         <v>136</v>
       </c>
       <c r="L55" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="N55" s="5" t="s">
         <v>136</v>
@@ -3560,11 +3578,11 @@
       <c r="O55" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P55" s="8" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+      <c r="P55" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="3" t="s">
         <v>25</v>
       </c>
@@ -3608,11 +3626,11 @@
       <c r="O56" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P56" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+      <c r="P56" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="3" t="s">
         <v>25</v>
       </c>
@@ -3645,10 +3663,10 @@
         <v>136</v>
       </c>
       <c r="L57" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="N57" s="5" t="s">
         <v>136</v>
@@ -3657,72 +3675,74 @@
         <v>136</v>
       </c>
       <c r="P57" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
+      <c r="A58" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I58" s="5">
+        <v>25</v>
+      </c>
+      <c r="J58" s="3"/>
+      <c r="K58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="N58" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P58" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="5"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="6"/>
-      <c r="P58" s="7"/>
-    </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
-      <c r="A59" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I59" s="5">
-        <v>25</v>
-      </c>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="5"/>
       <c r="J59" s="3"/>
       <c r="K59" s="5"/>
-      <c r="L59" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="M59" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="N59" s="5">
-        <v>2</v>
-      </c>
-      <c r="O59" s="6">
-        <v>5.09</v>
-      </c>
-      <c r="P59" s="7" t="s">
-        <v>183</v>
-      </c>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="6"/>
+      <c r="P59" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="3" t="s">
@@ -3764,7 +3784,7 @@
         <v>2</v>
       </c>
       <c r="O60" s="6">
-        <v>4.64</v>
+        <v>5.09</v>
       </c>
       <c r="P60" s="7" t="s">
         <v>186</v>
@@ -3796,7 +3816,7 @@
         <v>22</v>
       </c>
       <c r="I61" s="5">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="J61" s="3"/>
       <c r="K61" s="5"/>
@@ -3804,13 +3824,13 @@
         <v>187</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="N61" s="5">
-        <v>227</v>
-      </c>
-      <c r="O61" s="6" t="s">
-        <v>188</v>
+        <v>2</v>
+      </c>
+      <c r="O61" s="6">
+        <v>4.64</v>
       </c>
       <c r="P61" s="7" t="s">
         <v>189</v>
@@ -3850,13 +3870,13 @@
         <v>190</v>
       </c>
       <c r="M62" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N62" s="5">
+        <v>227</v>
+      </c>
+      <c r="O62" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="N62" s="5">
-        <v>17</v>
-      </c>
-      <c r="O62" s="6">
-        <v>5.09</v>
       </c>
       <c r="P62" s="7" t="s">
         <v>192</v>
@@ -3888,7 +3908,7 @@
         <v>22</v>
       </c>
       <c r="I63" s="5">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J63" s="3"/>
       <c r="K63" s="5"/>
@@ -3899,13 +3919,13 @@
         <v>194</v>
       </c>
       <c r="N63" s="5">
-        <v>51</v>
-      </c>
-      <c r="O63" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O63" s="6">
+        <v>5.09</v>
+      </c>
+      <c r="P63" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="P63" s="7" t="s">
-        <v>196</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
@@ -3913,7 +3933,7 @@
         <v>25</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>197</v>
+        <v>26</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>17</v>
@@ -3934,24 +3954,24 @@
         <v>22</v>
       </c>
       <c r="I64" s="5">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="J64" s="3"/>
       <c r="K64" s="5"/>
       <c r="L64" s="3" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="N64" s="5">
-        <v>20</v>
-      </c>
-      <c r="O64" s="6">
-        <v>3.85</v>
+        <v>51</v>
+      </c>
+      <c r="O64" s="6" t="s">
+        <v>198</v>
       </c>
       <c r="P64" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
@@ -3959,7 +3979,7 @@
         <v>25</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>17</v>
@@ -3985,38 +4005,66 @@
       <c r="J65" s="3"/>
       <c r="K65" s="5"/>
       <c r="L65" s="3" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
       <c r="N65" s="5">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="O65" s="6">
-        <v>91.1</v>
+        <v>3.85</v>
       </c>
       <c r="P65" s="7" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="5"/>
+      <c r="A66" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I66" s="5">
+        <v>25</v>
+      </c>
       <c r="J66" s="3"/>
       <c r="K66" s="5"/>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="5"/>
-      <c r="O66" s="6"/>
-      <c r="P66" s="7"/>
+      <c r="L66" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M66" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="N66" s="5">
+        <v>11</v>
+      </c>
+      <c r="O66" s="6">
+        <v>91.1</v>
+      </c>
+      <c r="P66" s="7" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="3"/>
@@ -4070,7 +4118,25 @@
       <c r="M69" s="3"/>
       <c r="N69" s="5"/>
       <c r="O69" s="6"/>
-      <c r="P69" s="6"/>
+      <c r="P69" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="3"/>
+      <c r="K70" s="5"/>
+      <c r="L70" s="3"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="5"/>
+      <c r="O70" s="6"/>
+      <c r="P70" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tested refractored code and added new job run, 8 batches is actually pretty good
</commit_message>
<xml_diff>
--- a/job_history.xlsx
+++ b/job_history.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="206">
   <si>
     <t>Data Used</t>
   </si>
@@ -512,6 +512,15 @@
   </si>
   <si>
     <t>22.2 &amp; 13.0</t>
+  </si>
+  <si>
+    <t>-65.7 &amp; -14.9</t>
+  </si>
+  <si>
+    <t>-11.8 &amp; -7.5</t>
+  </si>
+  <si>
+    <t>8 batches</t>
   </si>
   <si>
     <t>-18.5 &amp; -5</t>
@@ -1028,7 +1037,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -3390,7 +3399,7 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3" t="s">
         <v>25</v>
       </c>
@@ -3434,7 +3443,7 @@
       <c r="O52" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P52" s="7" t="s">
+      <c r="P52" s="8" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3486,7 +3495,7 @@
         <v>171</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="3" t="s">
         <v>25</v>
       </c>
@@ -3530,7 +3539,7 @@
       <c r="O54" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P54" s="8" t="s">
+      <c r="P54" s="7" t="s">
         <v>174</v>
       </c>
     </row>
@@ -3578,8 +3587,8 @@
       <c r="O55" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P55" s="7" t="s">
-        <v>154</v>
+      <c r="P55" s="9" t="s">
+        <v>177</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
@@ -3615,10 +3624,10 @@
         <v>136</v>
       </c>
       <c r="L56" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="N56" s="5" t="s">
         <v>136</v>
@@ -3626,8 +3635,8 @@
       <c r="O56" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="P56" s="9" t="s">
-        <v>179</v>
+      <c r="P56" s="7" t="s">
+        <v>154</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
@@ -3675,7 +3684,7 @@
         <v>136</v>
       </c>
       <c r="P57" s="7" t="s">
-        <v>151</v>
+        <v>182</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
@@ -3711,10 +3720,10 @@
         <v>136</v>
       </c>
       <c r="L58" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="N58" s="5" t="s">
         <v>136</v>
@@ -3723,72 +3732,74 @@
         <v>136</v>
       </c>
       <c r="P58" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
+      <c r="A59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I59" s="5">
+        <v>25</v>
+      </c>
+      <c r="J59" s="3"/>
+      <c r="K59" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="N59" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="P59" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="5"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="6"/>
-      <c r="P59" s="7"/>
-    </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
-      <c r="A60" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I60" s="5">
-        <v>25</v>
-      </c>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="5"/>
       <c r="J60" s="3"/>
       <c r="K60" s="5"/>
-      <c r="L60" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="M60" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="N60" s="5">
-        <v>2</v>
-      </c>
-      <c r="O60" s="6">
-        <v>5.09</v>
-      </c>
-      <c r="P60" s="7" t="s">
-        <v>186</v>
-      </c>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="6"/>
+      <c r="P60" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="3" t="s">
@@ -3830,7 +3841,7 @@
         <v>2</v>
       </c>
       <c r="O61" s="6">
-        <v>4.64</v>
+        <v>5.09</v>
       </c>
       <c r="P61" s="7" t="s">
         <v>189</v>
@@ -3862,7 +3873,7 @@
         <v>22</v>
       </c>
       <c r="I62" s="5">
-        <v>250</v>
+        <v>25</v>
       </c>
       <c r="J62" s="3"/>
       <c r="K62" s="5"/>
@@ -3870,13 +3881,13 @@
         <v>190</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="N62" s="5">
-        <v>227</v>
-      </c>
-      <c r="O62" s="6" t="s">
-        <v>191</v>
+        <v>2</v>
+      </c>
+      <c r="O62" s="6">
+        <v>4.64</v>
       </c>
       <c r="P62" s="7" t="s">
         <v>192</v>
@@ -3916,13 +3927,13 @@
         <v>193</v>
       </c>
       <c r="M63" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N63" s="5">
+        <v>227</v>
+      </c>
+      <c r="O63" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="N63" s="5">
-        <v>17</v>
-      </c>
-      <c r="O63" s="6">
-        <v>5.09</v>
       </c>
       <c r="P63" s="7" t="s">
         <v>195</v>
@@ -3954,7 +3965,7 @@
         <v>22</v>
       </c>
       <c r="I64" s="5">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="J64" s="3"/>
       <c r="K64" s="5"/>
@@ -3965,13 +3976,13 @@
         <v>197</v>
       </c>
       <c r="N64" s="5">
-        <v>51</v>
-      </c>
-      <c r="O64" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O64" s="6">
+        <v>5.09</v>
+      </c>
+      <c r="P64" s="7" t="s">
         <v>198</v>
-      </c>
-      <c r="P64" s="7" t="s">
-        <v>199</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
@@ -3979,7 +3990,7 @@
         <v>25</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>200</v>
+        <v>26</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>17</v>
@@ -4000,24 +4011,24 @@
         <v>22</v>
       </c>
       <c r="I65" s="5">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="J65" s="3"/>
       <c r="K65" s="5"/>
       <c r="L65" s="3" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="N65" s="5">
-        <v>20</v>
-      </c>
-      <c r="O65" s="6">
-        <v>3.85</v>
+        <v>51</v>
+      </c>
+      <c r="O65" s="6" t="s">
+        <v>201</v>
       </c>
       <c r="P65" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
@@ -4025,7 +4036,7 @@
         <v>25</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>17</v>
@@ -4051,38 +4062,66 @@
       <c r="J66" s="3"/>
       <c r="K66" s="5"/>
       <c r="L66" s="3" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="N66" s="5">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="O66" s="6">
-        <v>91.1</v>
+        <v>3.85</v>
       </c>
       <c r="P66" s="7" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="5"/>
+      <c r="A67" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I67" s="5">
+        <v>25</v>
+      </c>
       <c r="J67" s="3"/>
       <c r="K67" s="5"/>
-      <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
-      <c r="N67" s="5"/>
-      <c r="O67" s="6"/>
-      <c r="P67" s="7"/>
+      <c r="L67" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="M67" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="N67" s="5">
+        <v>11</v>
+      </c>
+      <c r="O67" s="6">
+        <v>91.1</v>
+      </c>
+      <c r="P67" s="7" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="3"/>
@@ -4136,7 +4175,25 @@
       <c r="M70" s="3"/>
       <c r="N70" s="5"/>
       <c r="O70" s="6"/>
-      <c r="P70" s="6"/>
+      <c r="P70" s="7"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+      <c r="A71" s="3"/>
+      <c r="B71" s="3"/>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="3"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="5"/>
+      <c r="J71" s="3"/>
+      <c r="K71" s="5"/>
+      <c r="L71" s="3"/>
+      <c r="M71" s="3"/>
+      <c r="N71" s="5"/>
+      <c r="O71" s="6"/>
+      <c r="P71" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>